<commit_message>
Clean up html structure and Update datastructure
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330" tabRatio="761"/>
+    <workbookView xWindow="120" yWindow="90" windowWidth="24915" windowHeight="12330" tabRatio="883"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="1" r:id="rId1"/>
@@ -14,25 +14,19 @@
     <sheet name="User_Orgs" sheetId="5" r:id="rId5"/>
     <sheet name="User_Relateds" sheetId="6" r:id="rId6"/>
     <sheet name="User_FitnessBasics" sheetId="7" r:id="rId7"/>
-    <sheet name="User_Videos" sheetId="8" r:id="rId8"/>
-    <sheet name="User_Images" sheetId="9" r:id="rId9"/>
-    <sheet name="User_PrimaryVideo" sheetId="10" r:id="rId10"/>
-    <sheet name="User_Commentsof" sheetId="11" r:id="rId11"/>
-    <sheet name="User_Commentson" sheetId="12" r:id="rId12"/>
-    <sheet name="User_CommentonForm" sheetId="13" r:id="rId13"/>
+    <sheet name="Media_Videos" sheetId="8" r:id="rId8"/>
+    <sheet name="Media_Images" sheetId="9" r:id="rId9"/>
+    <sheet name="Media_PrimaryVideo" sheetId="10" r:id="rId10"/>
+    <sheet name="SiteData_Commentsof" sheetId="11" r:id="rId11"/>
+    <sheet name="SiteData_Commentson" sheetId="12" r:id="rId12"/>
+    <sheet name="SiteData_CommentonForm" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="205">
-  <si>
-    <t>User Profile</t>
-  </si>
-  <si>
-    <t>Page</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="211">
   <si>
     <t>Model</t>
   </si>
@@ -415,21 +409,9 @@
     <t>user/collections/videos</t>
   </si>
   <si>
-    <t>Live Data : api/user/videos?user_id=101</t>
-  </si>
-  <si>
     <t>List of videos associated with the user.</t>
   </si>
   <si>
-    <t>test/user/videos/101</t>
-  </si>
-  <si>
-    <t>api/user/videos?user_id=101</t>
-  </si>
-  <si>
-    <t>Test Data : test/user/videos/101</t>
-  </si>
-  <si>
     <t>video_id</t>
   </si>
   <si>
@@ -490,21 +472,9 @@
     <t>List of images associated with the user.</t>
   </si>
   <si>
-    <t>api/user/images?user_id=101</t>
-  </si>
-  <si>
-    <t>test/user/images/101</t>
-  </si>
-  <si>
     <t>Image information</t>
   </si>
   <si>
-    <t>Live Data : api/user/images?user_id=101</t>
-  </si>
-  <si>
-    <t>Test Data : test/user/images/101</t>
-  </si>
-  <si>
     <t>image_id</t>
   </si>
   <si>
@@ -517,9 +487,6 @@
     <t>primaryvideo</t>
   </si>
   <si>
-    <t>user/models/primaryvideo</t>
-  </si>
-  <si>
     <t>Primary Video information about the user</t>
   </si>
   <si>
@@ -532,9 +499,6 @@
     <t>schedule</t>
   </si>
   <si>
-    <t>Live Data : api/user/primaryvideo?user_id=101</t>
-  </si>
-  <si>
     <t>Test Data : test/user/primaryvideo/101</t>
   </si>
   <si>
@@ -544,30 +508,15 @@
     <t>Primary Video information about the user.</t>
   </si>
   <si>
-    <t>api/user/primaryvideo?user_id=101</t>
-  </si>
-  <si>
-    <t>test/user/primaryvideo/101</t>
-  </si>
-  <si>
     <t>commentsof</t>
   </si>
   <si>
     <t>List of comments made by the user.</t>
   </si>
   <si>
-    <t>api/user/commentsof?user_id=101</t>
-  </si>
-  <si>
     <t>test/user/commentsof/101</t>
   </si>
   <si>
-    <t>Live Data : api/user/commentsof?user_id=101</t>
-  </si>
-  <si>
-    <t>Test Data : test/user/commentsof/101</t>
-  </si>
-  <si>
     <t>Comment information</t>
   </si>
   <si>
@@ -590,9 +539,6 @@
   </si>
   <si>
     <t>commentson</t>
-  </si>
-  <si>
-    <t>api/user/commentson?user_id=101</t>
   </si>
   <si>
     <t>test/user/commentson/101</t>
@@ -617,15 +563,6 @@
     <t>Leave comment ABOUT the user on his/her profile</t>
   </si>
   <si>
-    <t>Live Data : api/user/commentson?user_id=101</t>
-  </si>
-  <si>
-    <t>Test Data : test/user/commentson/101</t>
-  </si>
-  <si>
-    <t>api/user/commentsonform?user_id=101</t>
-  </si>
-  <si>
     <t>test/user/commentsonform/101</t>
   </si>
   <si>
@@ -635,12 +572,6 @@
     <t>user/models/commentonform</t>
   </si>
   <si>
-    <t>Live Data : api/user/commentonform?user_id=101</t>
-  </si>
-  <si>
-    <t>Test Data : test/user/commentonform/101</t>
-  </si>
-  <si>
     <t>Action: Get, Put</t>
   </si>
   <si>
@@ -648,6 +579,93 @@
   </si>
   <si>
     <t>commentonform</t>
+  </si>
+  <si>
+    <t>Packages</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Media</t>
+  </si>
+  <si>
+    <t>media/models/video</t>
+  </si>
+  <si>
+    <t>media/collections/videos</t>
+  </si>
+  <si>
+    <t>media/collections/images</t>
+  </si>
+  <si>
+    <t>media/models/image</t>
+  </si>
+  <si>
+    <t>media/models/primaryvideo</t>
+  </si>
+  <si>
+    <t>api/media/videos?user_id=101</t>
+  </si>
+  <si>
+    <t>api/media/images?user_id=101</t>
+  </si>
+  <si>
+    <t>test/media/videos/101</t>
+  </si>
+  <si>
+    <t>test/media/images/101</t>
+  </si>
+  <si>
+    <t>api/media/primaryvideo?user_id=101</t>
+  </si>
+  <si>
+    <t>test/media/primaryvideo/101</t>
+  </si>
+  <si>
+    <t>Test Data : test/media/videos/101</t>
+  </si>
+  <si>
+    <t>Test Data : test/media/images/101</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Live Data : </t>
+  </si>
+  <si>
+    <t>Site Data</t>
+  </si>
+  <si>
+    <t>sitedata/models/commentof</t>
+  </si>
+  <si>
+    <t>sitedata/models/commenton</t>
+  </si>
+  <si>
+    <t>sitedata/models/commentonform</t>
+  </si>
+  <si>
+    <t>sitedata/collections/commentsof</t>
+  </si>
+  <si>
+    <t>sitedata/collections/commentson</t>
+  </si>
+  <si>
+    <t>api/sitedata/commentsof?user_id=101</t>
+  </si>
+  <si>
+    <t>api/sitedata/commentson?user_id=101</t>
+  </si>
+  <si>
+    <t>api/sitedata/commentsonform?user_id=101</t>
+  </si>
+  <si>
+    <t>Test Data : test/sitedata/commentsof/101</t>
+  </si>
+  <si>
+    <t>Test Data : test/sitedata/commentson/101</t>
+  </si>
+  <si>
+    <t>Test Data : test/sitedata/commentonform/101</t>
   </si>
 </sst>
 </file>
@@ -881,21 +899,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -908,6 +914,39 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -916,12 +955,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -935,12 +968,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -949,15 +976,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1264,338 +1282,349 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D20" sqref="D20"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="17" customWidth="1"/>
-    <col min="2" max="2" width="16" style="17" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" style="17" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="17" customWidth="1"/>
-    <col min="5" max="5" width="47.85546875" style="17" customWidth="1"/>
-    <col min="6" max="6" width="38.140625" style="17" customWidth="1"/>
-    <col min="7" max="7" width="29.42578125" style="17" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="13" customWidth="1"/>
+    <col min="2" max="2" width="16" style="13" customWidth="1"/>
+    <col min="3" max="3" width="33.42578125" style="13" customWidth="1"/>
+    <col min="4" max="4" width="31.7109375" style="13" customWidth="1"/>
+    <col min="5" max="5" width="47.85546875" style="13" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="29.42578125" style="13" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="4" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" style="4" customWidth="1"/>
     <col min="10" max="10" width="8" style="4" customWidth="1"/>
     <col min="11" max="11" width="8.140625" style="4" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="17"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="19" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:11" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="C1" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="F1" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>183</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B3" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B4" s="16" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="I5" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="16" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>199</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>158</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>203</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>205</v>
+      </c>
+      <c r="G11" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B12" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>204</v>
+      </c>
+      <c r="E12" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>206</v>
+      </c>
+      <c r="G12" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B13" s="16" t="s">
+        <v>181</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>176</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>5</v>
-      </c>
-      <c r="F1" s="19" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>9</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="K1" s="6" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="20" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>168</v>
-      </c>
-      <c r="F2" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="C4" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D4" s="17" t="s">
-        <v>58</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>59</v>
-      </c>
-      <c r="G4" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>76</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="17" t="s">
-        <v>72</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>94</v>
-      </c>
-      <c r="D6" s="17" t="s">
-        <v>95</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="17" t="s">
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B14" s="16"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="E16" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="F16" s="13" t="s">
+        <v>190</v>
+      </c>
+      <c r="G16" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="I16" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="I6" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
-        <v>113</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>116</v>
-      </c>
-      <c r="E7" s="17" t="s">
-        <v>114</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>117</v>
-      </c>
-      <c r="G7" s="17" t="s">
-        <v>118</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>125</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="E8" s="17" t="s">
-        <v>128</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" s="17" t="s">
-        <v>129</v>
-      </c>
-      <c r="I8" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>149</v>
-      </c>
-      <c r="D9" s="17" t="s">
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B17" s="16" t="s">
+        <v>142</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>151</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>152</v>
-      </c>
-      <c r="G9" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="20" t="s">
-        <v>160</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>161</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>170</v>
-      </c>
-      <c r="G10" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="I10" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>172</v>
-      </c>
-      <c r="C11" s="17" t="s">
-        <v>188</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>190</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="G11" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="B12" s="20" t="s">
-        <v>185</v>
-      </c>
-      <c r="C12" s="17" t="s">
+      <c r="C18" s="13" t="s">
         <v>189</v>
       </c>
-      <c r="D12" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="E12" s="24" t="s">
-        <v>192</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>186</v>
-      </c>
-      <c r="G12" s="17" t="s">
-        <v>187</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>199</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="G13" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>14</v>
+      <c r="E18" s="13" t="s">
+        <v>157</v>
+      </c>
+      <c r="F18" s="13" t="s">
+        <v>194</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>195</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>99</v>
       </c>
     </row>
   </sheetData>
@@ -1606,12 +1635,12 @@
     <hyperlink ref="B5" location="User_Orgs!A1" display="orgs"/>
     <hyperlink ref="B6" location="User_Relateds!A1" display="relateds"/>
     <hyperlink ref="B7" location="User_FitnessBasics!A1" display="fitnessbasics"/>
-    <hyperlink ref="B8" location="User_Videos!A1" display="videos"/>
-    <hyperlink ref="B9" location="User_Images!A1" display="images"/>
-    <hyperlink ref="B10" location="User_PrimaryVideo!A1" display="primaryvideo"/>
-    <hyperlink ref="B11" location="User_Commentsof!A1" display="commentsof"/>
-    <hyperlink ref="B12" location="User_Commentson!A1" display="commentson"/>
-    <hyperlink ref="B13" location="User_CommentonForm!A1" display="commentform"/>
+    <hyperlink ref="B16" location="Media_Videos!A1" display="videos"/>
+    <hyperlink ref="B17" location="Media_Images!A1" display="images"/>
+    <hyperlink ref="B18" location="Media_PrimaryVideo!A1" display="primaryvideo"/>
+    <hyperlink ref="B11" location="SiteData_Commentsof!A1" display="commentsof"/>
+    <hyperlink ref="B12" location="SiteData_Commentson!A1" display="commentson"/>
+    <hyperlink ref="B13" location="SiteData_CommentonForm!A1" display="commentonform"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1623,7 +1652,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1638,57 +1667,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>161</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
-        <v>167</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
+        <v>155</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="8">
         <v>0</v>
@@ -1696,153 +1725,153 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="E12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D18" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D19" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="E23" t="s">
         <v>24</v>
-      </c>
-      <c r="E23" t="s">
-        <v>26</v>
       </c>
       <c r="F23" s="8">
         <v>0</v>
@@ -1850,10 +1879,10 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F24" s="8">
         <v>0</v>
@@ -1861,10 +1890,10 @@
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F25" s="8">
         <v>0</v>
@@ -1872,29 +1901,29 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F27" s="9" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F30" s="8">
         <v>0</v>
@@ -1902,10 +1931,10 @@
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F31" s="8" t="b">
         <v>0</v>
@@ -1931,7 +1960,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F26" sqref="F26"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1944,44 +1973,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -1989,73 +2018,73 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="E8" t="s">
-        <v>184</v>
+        <v>167</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>178</v>
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -2063,10 +2092,10 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F14" s="8" t="b">
         <v>0</v>
@@ -2074,72 +2103,72 @@
     </row>
     <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="21" t="s">
-        <v>190</v>
-      </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="B17" s="28" t="s">
+        <v>172</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>176</v>
-      </c>
-      <c r="B18" s="10"/>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="F18" s="12"/>
-      <c r="G18" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="F18" s="26"/>
+      <c r="G18" s="11"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="15"/>
+      <c r="E20" s="12"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F24" s="8">
         <v>0</v>
@@ -2147,10 +2176,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F25" s="8" t="b">
         <v>0</v>
@@ -2177,7 +2206,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B1"/>
+      <selection pane="bottomLeft" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2186,221 +2215,221 @@
     <col min="2" max="2" width="15" style="3" customWidth="1"/>
     <col min="3" max="4" width="9.140625" style="3"/>
     <col min="5" max="5" width="13.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.28515625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>189</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="30" t="s">
-        <v>41</v>
+        <v>13</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="17">
+        <v>24</v>
+      </c>
+      <c r="F4" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>29</v>
+        <v>167</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>178</v>
+        <v>17</v>
+      </c>
+      <c r="F10" s="20" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F13" s="17">
+        <v>30</v>
+      </c>
+      <c r="F13" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F14" s="17" t="b">
+        <v>32</v>
+      </c>
+      <c r="F14" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="B17" s="27" t="s">
-        <v>191</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="29"/>
+        <v>71</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="34"/>
       <c r="E17" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F17" s="19" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="F17" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="32" t="s">
-        <v>194</v>
-      </c>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="33" t="s">
-        <v>195</v>
-      </c>
-      <c r="F18" s="34"/>
-      <c r="G18" s="35"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="35" t="s">
+        <v>198</v>
+      </c>
+      <c r="B18" s="35"/>
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="36" t="s">
+        <v>209</v>
+      </c>
+      <c r="F18" s="37"/>
+      <c r="G18" s="21"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>47</v>
+        <v>13</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="37"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="25" t="s">
-        <v>192</v>
+        <v>17</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F24" s="17">
+        <v>30</v>
+      </c>
+      <c r="F24" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F25" s="17" t="b">
+        <v>32</v>
+      </c>
+      <c r="F25" s="13" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2435,174 +2464,174 @@
     <col min="3" max="3" width="9.140625" style="3"/>
     <col min="4" max="4" width="13" style="3" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="3" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="62.28515625" style="3" customWidth="1"/>
     <col min="8" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="31"/>
     </row>
     <row r="2" spans="1:7" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>199</v>
-      </c>
-      <c r="C2" s="28"/>
-      <c r="D2" s="29"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="32" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="33"/>
+      <c r="D2" s="34"/>
       <c r="E2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="19" t="s">
-        <v>28</v>
+        <v>20</v>
+      </c>
+      <c r="F2" s="15" t="s">
+        <v>26</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
-        <v>201</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="14" t="s">
-        <v>202</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="11" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="30" t="s">
-        <v>41</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>179</v>
+        <v>162</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="17">
+        <v>24</v>
+      </c>
+      <c r="F6" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>180</v>
+        <v>163</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="3" t="s">
-        <v>203</v>
+        <v>180</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>181</v>
+        <v>164</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F9" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F10" s="17" t="s">
-        <v>29</v>
+        <v>17</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="3" t="s">
-        <v>183</v>
+        <v>166</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="F11" s="17" t="s">
-        <v>29</v>
+        <v>167</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F13" s="31" t="s">
-        <v>198</v>
+        <v>17</v>
+      </c>
+      <c r="F13" s="20" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="F16" s="17">
+        <v>30</v>
+      </c>
+      <c r="F16" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F17" s="17" t="b">
+        <v>32</v>
+      </c>
+      <c r="F17" s="13" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E20" s="37"/>
+      <c r="E20" s="23"/>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="E21" s="37"/>
+      <c r="E21" s="23"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="F22" s="25"/>
+      <c r="F22" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -2637,103 +2666,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="F3" s="12"/>
-      <c r="G3" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" s="26"/>
+      <c r="G3" s="11"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -2741,10 +2770,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
         <v>24</v>
-      </c>
-      <c r="E12" t="s">
-        <v>26</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -2752,32 +2781,32 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B14" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F17" s="8">
         <v>0</v>
@@ -2785,10 +2814,10 @@
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E18" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F18" s="8" t="b">
         <v>0</v>
@@ -2827,140 +2856,140 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>36</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>34</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" t="s">
-        <v>47</v>
-      </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
@@ -2968,10 +2997,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F17" s="8" t="b">
         <v>0</v>
@@ -2979,69 +3008,69 @@
     </row>
     <row r="20" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="C20" s="22"/>
-      <c r="D20" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="B20" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
       <c r="E20" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="10"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="F21" s="12"/>
-      <c r="G21" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
+      <c r="D21" s="24"/>
+      <c r="E21" s="25" t="s">
+        <v>51</v>
+      </c>
+      <c r="F21" s="26"/>
+      <c r="G21" s="11"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F27" s="8">
         <v>0</v>
@@ -3049,10 +3078,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F28" s="8" t="b">
         <v>0</v>
@@ -3092,85 +3121,85 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F10" s="8">
         <v>0</v>
@@ -3178,10 +3207,10 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E11" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F11" s="8" t="b">
         <v>0</v>
@@ -3189,72 +3218,72 @@
     </row>
     <row r="14" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>58</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
       <c r="E14" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="10"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="11" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="F15" s="26"/>
+      <c r="G15" s="11"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E17" s="15"/>
+      <c r="E17" s="12"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F21" s="8">
         <v>0</v>
@@ -3262,10 +3291,10 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E22" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F22" s="8" t="b">
         <v>0</v>
@@ -3307,77 +3336,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="8">
         <v>0</v>
@@ -3385,54 +3414,54 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F14" s="8">
         <v>0</v>
@@ -3440,73 +3469,73 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D15" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D16" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F17" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D22" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E23" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F23" s="8">
         <v>0</v>
@@ -3514,29 +3543,29 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E28" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F28" s="8">
         <v>0</v>
@@ -3544,10 +3573,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E29" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F29" s="8" t="b">
         <v>0</v>
@@ -3555,69 +3584,69 @@
     </row>
     <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+      <c r="E32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B32" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="C32" s="22"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="B33" s="10"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="10"/>
-      <c r="E33" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="F33" s="12"/>
-      <c r="G33" s="14"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="11"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B36" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E36" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E39" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F39" s="8">
         <v>0</v>
@@ -3625,10 +3654,10 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E40" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F40" s="8" t="b">
         <v>0</v>
@@ -3668,44 +3697,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -3713,98 +3742,98 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" t="s">
         <v>24</v>
-      </c>
-      <c r="E14" t="s">
-        <v>26</v>
       </c>
       <c r="F14" s="8">
         <v>0</v>
@@ -3812,10 +3841,10 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E15" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -3823,29 +3852,29 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E17" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F20" s="8">
         <v>0</v>
@@ -3853,10 +3882,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F21" s="8" t="b">
         <v>0</v>
@@ -3864,72 +3893,72 @@
     </row>
     <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="B24" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+      <c r="E24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B25" s="24"/>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="22"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G24" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="10" t="s">
-        <v>96</v>
-      </c>
-      <c r="B25" s="10"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="F25" s="12"/>
-      <c r="G25" s="14"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="11"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E27" s="15"/>
+      <c r="E27" s="12"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E31" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F31" s="8">
         <v>0</v>
@@ -3937,10 +3966,10 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E32" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F32" s="8" t="b">
         <v>0</v>
@@ -3982,96 +4011,96 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F11" s="8">
         <v>0</v>
@@ -4079,10 +4108,10 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E12" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F12" s="8" t="b">
         <v>0</v>
@@ -4090,69 +4119,69 @@
     </row>
     <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>116</v>
-      </c>
-      <c r="C15" s="22"/>
-      <c r="D15" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B16" s="10"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="G16" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>117</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="25" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="26"/>
+      <c r="G16" s="11"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F22" s="8">
         <v>0</v>
@@ -4160,10 +4189,10 @@
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F23" s="8" t="b">
         <v>0</v>
@@ -4190,7 +4219,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G24" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4203,44 +4232,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -4248,98 +4277,98 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E8" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="E9" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="E13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F13" s="8">
         <v>0</v>
@@ -4347,21 +4376,21 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="E14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="F14" s="8" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15" t="s">
         <v>24</v>
-      </c>
-      <c r="E15" t="s">
-        <v>26</v>
       </c>
       <c r="F15" s="8">
         <v>0</v>
@@ -4369,10 +4398,10 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F16" s="8">
         <v>0</v>
@@ -4380,10 +4409,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="E17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F17" s="8">
         <v>0</v>
@@ -4391,29 +4420,29 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F22" s="8">
         <v>0</v>
@@ -4421,10 +4450,10 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E23" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F23" s="8" t="b">
         <v>0</v>
@@ -4432,72 +4461,72 @@
     </row>
     <row r="26" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C26" s="22"/>
-      <c r="D26" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="B26" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
       <c r="E26" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G26" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11" t="s">
-        <v>131</v>
-      </c>
-      <c r="F27" s="12"/>
-      <c r="G27" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="25" t="s">
+        <v>196</v>
+      </c>
+      <c r="F27" s="26"/>
+      <c r="G27" s="11"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E29" s="15"/>
+      <c r="E29" s="12"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B30" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E33" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F33" s="8">
         <v>0</v>
@@ -4505,10 +4534,10 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E34" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F34" s="8" t="b">
         <v>0</v>
@@ -4535,7 +4564,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G30" sqref="A1:XFD1048576"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4548,44 +4577,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="16"/>
+      <c r="A1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>149</v>
-      </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="23"/>
+        <v>0</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F4" s="8">
         <v>0</v>
@@ -4593,32 +4622,32 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
-      </c>
-      <c r="E7" t="s">
-        <v>26</v>
       </c>
       <c r="F7" s="8">
         <v>0</v>
@@ -4626,29 +4655,29 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F12" s="8">
         <v>0</v>
@@ -4656,10 +4685,10 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E13" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F13" s="8" t="b">
         <v>0</v>
@@ -4667,72 +4696,72 @@
     </row>
     <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B16" s="21" t="s">
-        <v>150</v>
-      </c>
-      <c r="C16" s="22"/>
-      <c r="D16" s="23"/>
+        <v>71</v>
+      </c>
+      <c r="B16" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
       <c r="E16" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="10" t="s">
-        <v>155</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="11" t="s">
-        <v>156</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="G17" s="14"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="24" t="s">
+        <v>198</v>
+      </c>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="F17" s="26"/>
+      <c r="G17" s="11"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E19" s="15"/>
+      <c r="E19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F23" s="8">
         <v>0</v>
@@ -4740,10 +4769,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="F24" s="8" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
Add Game Page Header and Rosters(#153, #159, #164, #166)
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="3"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -24,17 +24,18 @@
     <sheet name="Sportorg_Teams" sheetId="24" r:id="rId15"/>
     <sheet name="Sportorg_Games" sheetId="25" r:id="rId16"/>
     <sheet name="Sportorg_Matches" sheetId="26" r:id="rId17"/>
-    <sheet name="Sportorg_Seasons" sheetId="27" r:id="rId18"/>
-    <sheet name="Media_Videos" sheetId="8" r:id="rId19"/>
-    <sheet name="Media_Images" sheetId="9" r:id="rId20"/>
-    <sheet name="Media_VideoService" sheetId="19" r:id="rId21"/>
+    <sheet name="Sportorg_TeamRosters" sheetId="28" r:id="rId18"/>
+    <sheet name="Sportorg_Seasons" sheetId="27" r:id="rId19"/>
+    <sheet name="Media_Videos" sheetId="8" r:id="rId20"/>
+    <sheet name="Media_Images" sheetId="9" r:id="rId21"/>
+    <sheet name="Media_VideoService" sheetId="19" r:id="rId22"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1056" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="324">
   <si>
     <t>User Profile</t>
   </si>
@@ -929,13 +930,100 @@
   </si>
   <si>
     <t>sportorg/collections/complevels</t>
+  </si>
+  <si>
+    <t>Game</t>
+  </si>
+  <si>
+    <t>game/models/basics</t>
+  </si>
+  <si>
+    <t>Basic information about the game</t>
+  </si>
+  <si>
+    <t>api/game/basics?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/basics/101</t>
+  </si>
+  <si>
+    <t>game_name</t>
+  </si>
+  <si>
+    <t>game_picture</t>
+  </si>
+  <si>
+    <t>team_name</t>
+  </si>
+  <si>
+    <t>team_location</t>
+  </si>
+  <si>
+    <t>points_scored</t>
+  </si>
+  <si>
+    <t>game_location</t>
+  </si>
+  <si>
+    <t>id, game_name, game_day, game_time</t>
+  </si>
+  <si>
+    <t>game_picture, teams(team_name, tema_location, points_scored), game_location</t>
+  </si>
+  <si>
+    <t>added fields</t>
+  </si>
+  <si>
+    <t>teamrosters</t>
+  </si>
+  <si>
+    <t>game/collections/teamrosters</t>
+  </si>
+  <si>
+    <t>sportorg/collections/teamrosters</t>
+  </si>
+  <si>
+    <t>Team Rosters associated with the game</t>
+  </si>
+  <si>
+    <t>api/game/teamrosters?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/teamrosters/101</t>
+  </si>
+  <si>
+    <t>List of team rosters</t>
+  </si>
+  <si>
+    <t>Team Rosters information</t>
+  </si>
+  <si>
+    <t>packages/sportorg/models/teamroster</t>
+  </si>
+  <si>
+    <t>team_id</t>
+  </si>
+  <si>
+    <t>rosters</t>
+  </si>
+  <si>
+    <t>picture</t>
+  </si>
+  <si>
+    <t>sport_type</t>
+  </si>
+  <si>
+    <t>packages/sportorg/collections/teamrosters</t>
+  </si>
+  <si>
+    <t>sportorg/models/teamroster</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -981,8 +1069,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -997,6 +1092,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -1070,14 +1170,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1121,6 +1222,13 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1137,9 +1245,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="5" builtinId="27"/>
     <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
@@ -1446,10 +1554,10 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1467,10 +1575,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="16" t="s">
         <v>135</v>
       </c>
@@ -1665,7 +1773,15 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="17"/>
+      <c r="B18" s="17" t="s">
+        <v>309</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="17"/>
@@ -1796,6 +1912,7 @@
     <hyperlink ref="B17" location="Sportorg_Seasons!A1" display="seasons"/>
     <hyperlink ref="B13" location="Sportorg_Orgs!A1" display="orgs"/>
     <hyperlink ref="B12" location="Sportorg_Complevels!A1" display="complevels"/>
+    <hyperlink ref="B18" location="Sportorg_TeamRosters!A1" display="teamrosters"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1821,14 +1938,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -1837,11 +1954,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1960,11 +2077,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2047,7 +2164,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="A1:XFD1048576"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2063,14 +2180,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2079,11 +2196,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2202,11 +2319,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2305,14 +2422,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2321,11 +2438,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2455,11 +2572,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2558,14 +2675,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2574,11 +2691,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2686,11 +2803,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>291</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2795,14 +2912,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -2811,11 +2928,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2867,7 +2984,7 @@
       <c r="B7" s="20" t="s">
         <v>250</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>36</v>
       </c>
       <c r="F7" s="6"/>
@@ -2965,11 +3082,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3068,14 +3185,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3084,11 +3201,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>257</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3138,7 +3255,7 @@
       <c r="B7" s="20" t="s">
         <v>56</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3219,11 +3336,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="28" t="s">
         <v>258</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3303,17 +3420,17 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" style="20" customWidth="1"/>
     <col min="2" max="2" width="17" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="20"/>
+    <col min="3" max="3" width="13.7109375" style="20" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" style="20" customWidth="1"/>
     <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
     <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
@@ -3322,27 +3439,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
-        <v>41352</v>
+        <v>41353</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3372,17 +3489,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>14</v>
-      </c>
+    <row r="5" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>14</v>
@@ -3390,122 +3508,198 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="E7" s="27" t="s">
+        <v>267</v>
+      </c>
+      <c r="E7" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="20" t="s">
+        <v>301</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="20" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" s="22" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="20" t="s">
+        <v>302</v>
+      </c>
+      <c r="E10" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="20" t="s">
+        <v>303</v>
+      </c>
+      <c r="E11" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C12" s="20" t="s">
+        <v>304</v>
+      </c>
+      <c r="E12" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>305</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B15" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="E15" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="7" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="20" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E18" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E19" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
+      <c r="F19" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B22" s="28" t="s">
         <v>258</v>
       </c>
-      <c r="C21" s="24"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="2" t="s">
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+      <c r="E22" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F21" s="5" t="s">
+      <c r="F22" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G21" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="8"/>
-    </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B25" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="7" t="s">
+      <c r="E25" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F25" s="7" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="20" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="E27" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F27" s="6">
-        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B28" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E28" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E29" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="6" t="b">
-        <v>0</v>
+      <c r="F29" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>132</v>
+      </c>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="14">
+        <v>41352</v>
+      </c>
+      <c r="B33" s="20" t="s">
+        <v>308</v>
+      </c>
+      <c r="C33" s="20" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="14">
+        <v>41353</v>
+      </c>
+      <c r="B34" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="C34" s="20" t="s">
+        <v>307</v>
       </c>
     </row>
   </sheetData>
@@ -3513,7 +3707,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
@@ -3544,14 +3738,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3560,11 +3754,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3614,7 +3808,7 @@
       <c r="B7" s="20" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="27" t="s">
+      <c r="E7" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3622,7 +3816,7 @@
       <c r="B8" s="20" t="s">
         <v>278</v>
       </c>
-      <c r="E8" s="27" t="s">
+      <c r="E8" s="22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -3630,7 +3824,7 @@
       <c r="C9" s="20" t="s">
         <v>279</v>
       </c>
-      <c r="E9" s="27" t="s">
+      <c r="E9" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3703,11 +3897,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="28" t="s">
         <v>275</v>
       </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -3790,30 +3984,30 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="17" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="20"/>
-    <col min="4" max="4" width="12.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="23" customWidth="1"/>
     <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="20"/>
+    <col min="7" max="7" width="62.28515625" style="23" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3822,11 +4016,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>286</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="28" t="s">
+        <v>317</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3838,7 +4032,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -3846,54 +4040,78 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>169</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>289</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>14</v>
+      <c r="B5" s="23" t="s">
+        <v>302</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="27"/>
+      <c r="C7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="27"/>
+      <c r="C8" s="23" t="s">
+        <v>320</v>
+      </c>
+      <c r="E8" s="22"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="27"/>
+      <c r="C9" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E9" s="22"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="23" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="23" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>288</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="23" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="6">
@@ -3901,10 +4119,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F20" s="6" t="b">
@@ -3915,11 +4133,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="23" t="s">
-        <v>287</v>
-      </c>
-      <c r="C23" s="24"/>
-      <c r="D23" s="25"/>
+      <c r="B23" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -3931,7 +4149,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -3942,29 +4160,29 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>290</v>
+        <v>315</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="23" t="s">
         <v>27</v>
       </c>
       <c r="F29" s="6">
@@ -3972,10 +4190,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="6" t="b">
@@ -3999,41 +4217,46 @@
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="17" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="20"/>
+    <col min="4" max="4" width="12.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
     <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="20" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="20"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="14">
+        <v>41352</v>
+      </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="B2" s="28" t="s">
+        <v>286</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4045,291 +4268,160 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F3"/>
+      <c r="A3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="B4" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>289</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="22"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E6" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>92</v>
-      </c>
-      <c r="E7" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>93</v>
-      </c>
-      <c r="E8" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>40</v>
-      </c>
-      <c r="E9" t="s">
-        <v>101</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
-        <v>21</v>
-      </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
-        <v>21</v>
-      </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" t="s">
-        <v>21</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="E24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B26" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E26" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E29" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E30" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B27" s="23" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G27" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>22</v>
-      </c>
-      <c r="B31" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
-        <v>26</v>
-      </c>
-      <c r="E34" t="s">
-        <v>27</v>
-      </c>
-      <c r="F34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
-        <v>28</v>
-      </c>
-      <c r="E35" t="s">
-        <v>29</v>
-      </c>
-      <c r="F35" s="6" t="b">
+      <c r="F30" s="6" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B23:D23"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A1:B1" location="Packages!A1" display="Table of Contents"/>
-    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages!A1"/>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4337,13 +4429,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L14"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4363,10 +4455,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="21"/>
+      <c r="B1" s="26"/>
       <c r="C1" s="16" t="s">
         <v>135</v>
       </c>
@@ -4689,6 +4781,55 @@
       </c>
       <c r="K14" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>296</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>312</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>314</v>
       </c>
     </row>
   </sheetData>
@@ -4708,12 +4849,352 @@
     <hyperlink ref="E6" location="Sportorg_Orgs!A1" display="sportorg/collections/orgs"/>
     <hyperlink ref="E5" location="Sportorg_Teams!A1" display="sportorg/collections/teams"/>
     <hyperlink ref="E4" location="Sportorg_Sports!A1" display="sportorg/collections/sports"/>
+    <hyperlink ref="E16" location="Sportorg_Games!A1" display="sportorg/models/game"/>
+    <hyperlink ref="E17" location="Sportorg_TeamRosters!A1" display="sportorg/collections/teamrosters"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G40" sqref="G40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" s="27"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
+        <v>101</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>97</v>
+      </c>
+      <c r="E14" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>98</v>
+      </c>
+      <c r="E15" t="s">
+        <v>101</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+      <c r="F16" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>99</v>
+      </c>
+      <c r="E17" t="s">
+        <v>21</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>100</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F28"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="8"/>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>26</v>
+      </c>
+      <c r="E34" t="s">
+        <v>27</v>
+      </c>
+      <c r="F34" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" t="s">
+        <v>29</v>
+      </c>
+      <c r="F35" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Table of Contents"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages!A1"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -4731,24 +5212,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4857,11 +5338,11 @@
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C17" s="24"/>
-      <c r="D17" s="25"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -4873,12 +5354,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="26"/>
-      <c r="B18" s="26"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="26"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="26"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -4947,7 +5428,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -4979,14 +5460,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>206</v>
@@ -4996,11 +5477,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5176,7 +5657,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
@@ -5191,18 +5672,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5387,11 +5868,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="23" t="s">
+      <c r="B24" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="C24" s="24"/>
-      <c r="D24" s="25"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -5485,18 +5966,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22"/>
-      <c r="B1" s="22"/>
+      <c r="A1" s="27"/>
+      <c r="B1" s="27"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5593,11 +6074,11 @@
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="C15" s="24"/>
-      <c r="D15" s="25"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -5686,14 +6167,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -5702,11 +6183,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5850,11 +6331,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>212</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -5952,14 +6433,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -5968,11 +6449,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>214</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6091,11 +6572,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6211,14 +6692,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6227,11 +6708,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6339,11 +6820,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6441,14 +6922,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22" t="s">
+      <c r="B1" s="27"/>
+      <c r="C1" s="27" t="s">
         <v>135</v>
       </c>
-      <c r="D1" s="22"/>
+      <c r="D1" s="27"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6457,11 +6938,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="30"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6580,11 +7061,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="C19" s="24"/>
-      <c r="D19" s="25"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
add game page - video player
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="13" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="334">
   <si>
     <t>User Profile</t>
   </si>
@@ -347,12 +347,6 @@
     <t>string array</t>
   </si>
   <si>
-    <t>null (ex: "team1", "team2", etc)</t>
-  </si>
-  <si>
-    <t>null (ex: "game1", "game2", etc)</t>
-  </si>
-  <si>
     <t>null (ex: "tag1", "tag2", etc)</t>
   </si>
   <si>
@@ -1017,6 +1011,42 @@
   </si>
   <si>
     <t>sportorg/models/teamroster</t>
+  </si>
+  <si>
+    <t>videoplayer</t>
+  </si>
+  <si>
+    <t>game/models/videoplayer</t>
+  </si>
+  <si>
+    <t>Video player in game page</t>
+  </si>
+  <si>
+    <t>api/game/videoplayer?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/videoplayer/101</t>
+  </si>
+  <si>
+    <t>change teams, games variable</t>
+  </si>
+  <si>
+    <t>schedule</t>
+  </si>
+  <si>
+    <t>schedule_date</t>
+  </si>
+  <si>
+    <t>other_team</t>
+  </si>
+  <si>
+    <t>schedule_summary</t>
+  </si>
+  <si>
+    <t>team1_name</t>
+  </si>
+  <si>
+    <t>team2_name</t>
   </si>
 </sst>
 </file>
@@ -1178,7 +1208,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1229,6 +1259,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1575,26 +1606,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="27"/>
       <c r="C1" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>4</v>
@@ -1614,7 +1645,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B3" s="17" t="s">
         <v>3</v>
@@ -1683,38 +1714,38 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B10" s="17" t="s">
         <v>20</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="D11" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1722,10 +1753,10 @@
         <v>46</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -1733,10 +1764,10 @@
         <v>40</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1744,43 +1775,43 @@
         <v>94</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
+        <v>269</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>270</v>
+      </c>
+      <c r="D16" s="9" t="s">
         <v>271</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>272</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>273</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
+        <v>281</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="9" t="s">
         <v>283</v>
-      </c>
-      <c r="C17" s="9" t="s">
-        <v>284</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="D18" s="9" t="s">
         <v>309</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1791,27 +1822,27 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
+        <v>163</v>
+      </c>
+      <c r="B21" s="17" t="s">
+        <v>164</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="B21" s="17" t="s">
-        <v>166</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>167</v>
-      </c>
       <c r="D21" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
+        <v>174</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="9" t="s">
         <v>176</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>178</v>
       </c>
       <c r="E22" s="13"/>
     </row>
@@ -1820,33 +1851,33 @@
         <v>98</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>192</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>199</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1854,35 +1885,35 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B28" s="17" t="s">
         <v>86</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="17" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1938,14 +1969,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -1954,11 +1985,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>219</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>217</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -1979,7 +2010,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -1990,7 +2021,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>14</v>
@@ -2001,7 +2032,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>14</v>
@@ -2012,7 +2043,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>14</v>
@@ -2023,7 +2054,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
@@ -2043,7 +2074,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2077,11 +2108,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2114,7 +2145,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2180,14 +2211,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2196,11 +2227,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>222</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2221,7 +2252,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -2243,7 +2274,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>29</v>
@@ -2254,7 +2285,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>29</v>
@@ -2265,7 +2296,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
@@ -2319,11 +2350,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>223</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2356,7 +2387,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2422,14 +2453,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2438,11 +2469,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2463,7 +2494,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -2496,7 +2527,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>21</v>
@@ -2507,7 +2538,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
@@ -2518,7 +2549,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>14</v>
@@ -2538,7 +2569,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2572,11 +2603,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2609,7 +2640,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2675,14 +2706,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2691,11 +2722,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>239</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2716,7 +2747,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>21</v>
@@ -2738,7 +2769,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="19" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="E6" s="19" t="s">
         <v>21</v>
@@ -2749,7 +2780,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="19" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>21</v>
@@ -2769,7 +2800,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2803,11 +2834,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>291</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2842,7 +2873,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="23" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
@@ -2912,14 +2943,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -2928,11 +2959,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>247</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2953,7 +2984,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="19" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="19" t="s">
         <v>21</v>
@@ -2982,7 +3013,7 @@
     </row>
     <row r="7" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>36</v>
@@ -2991,7 +3022,7 @@
     </row>
     <row r="8" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E8" s="20" t="s">
         <v>36</v>
@@ -3000,7 +3031,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>14</v>
@@ -3011,7 +3042,7 @@
     </row>
     <row r="10" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>36</v>
@@ -3020,7 +3051,7 @@
     </row>
     <row r="11" spans="1:7" s="20" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>14</v>
@@ -3082,11 +3113,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>248</v>
-      </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
+      <c r="B21" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3119,7 +3150,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3185,14 +3216,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3201,11 +3232,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>255</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3226,7 +3257,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>21</v>
@@ -3269,7 +3300,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="20" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="E9" s="20" t="s">
         <v>14</v>
@@ -3277,7 +3308,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>14</v>
@@ -3285,7 +3316,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B11" s="20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>38</v>
@@ -3336,11 +3367,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="30"/>
+      <c r="B21" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C21" s="30"/>
+      <c r="D21" s="31"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3373,7 +3404,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3439,14 +3470,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -3455,11 +3486,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>265</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>263</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3480,7 +3511,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>21</v>
@@ -3491,7 +3522,7 @@
     </row>
     <row r="5" spans="1:7" s="21" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B5" s="21" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="E5" s="21" t="s">
         <v>14</v>
@@ -3500,7 +3531,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>14</v>
@@ -3508,7 +3539,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E7" s="20" t="s">
         <v>14</v>
@@ -3516,7 +3547,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>14</v>
@@ -3532,7 +3563,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>14</v>
@@ -3540,7 +3571,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>14</v>
@@ -3548,7 +3579,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>21</v>
@@ -3556,7 +3587,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" s="20" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>14</v>
@@ -3573,7 +3604,7 @@
         <v>14</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -3607,11 +3638,11 @@
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="28" t="s">
-        <v>258</v>
-      </c>
-      <c r="C22" s="29"/>
-      <c r="D22" s="30"/>
+      <c r="B22" s="29" t="s">
+        <v>256</v>
+      </c>
+      <c r="C22" s="30"/>
+      <c r="D22" s="31"/>
       <c r="E22" s="2" t="s">
         <v>17</v>
       </c>
@@ -3644,7 +3675,7 @@
         <v>14</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -3676,7 +3707,7 @@
     </row>
     <row r="32" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="F32" s="25"/>
     </row>
@@ -3685,10 +3716,10 @@
         <v>41352</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
@@ -3696,10 +3727,10 @@
         <v>41353</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="C34" s="20" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -3738,14 +3769,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3754,11 +3785,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>274</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>272</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3779,7 +3810,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>21</v>
@@ -3790,7 +3821,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>14</v>
@@ -3798,7 +3829,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="20" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="E6" s="20" t="s">
         <v>14</v>
@@ -3806,7 +3837,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="20" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>14</v>
@@ -3814,7 +3845,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="20" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>38</v>
@@ -3822,7 +3853,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>14</v>
@@ -3830,7 +3861,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="20" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="E10" s="20" t="s">
         <v>21</v>
@@ -3838,7 +3869,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="20" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="E11" s="20" t="s">
         <v>14</v>
@@ -3846,7 +3877,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="20" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="E12" s="20" t="s">
         <v>29</v>
@@ -3863,7 +3894,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -3897,11 +3928,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>275</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="B23" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -3934,7 +3965,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -3984,7 +4015,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4000,14 +4031,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4016,11 +4047,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>317</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4041,7 +4072,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>21</v>
@@ -4049,7 +4080,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="23" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="E5" s="23" t="s">
         <v>14</v>
@@ -4057,36 +4088,51 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>319</v>
+        <v>317</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="E7" s="22"/>
+      <c r="E7" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" s="23" t="s">
-        <v>320</v>
-      </c>
-      <c r="E8" s="22"/>
+        <v>318</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C9" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="E9" s="22"/>
+        <v>129</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="23" t="s">
-        <v>321</v>
+        <v>319</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="23" t="s">
         <v>37</v>
       </c>
+      <c r="E11" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="23" t="s">
@@ -4099,7 +4145,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4133,11 +4179,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>322</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="B23" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4170,7 +4216,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4236,14 +4282,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4252,11 +4298,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>286</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4277,7 +4323,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>21</v>
@@ -4285,7 +4331,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="20" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="E5" s="20" t="s">
         <v>14</v>
@@ -4311,7 +4357,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4345,11 +4391,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="28" t="s">
-        <v>287</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30"/>
+      <c r="B23" s="29" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" s="30"/>
+      <c r="D23" s="31"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4382,7 +4428,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4429,13 +4475,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L17"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4455,29 +4501,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="26"/>
+      <c r="A1" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="27"/>
       <c r="C1" s="16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:12" s="11" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D2" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="10" t="s">
         <v>148</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>150</v>
       </c>
       <c r="F2" s="11" t="s">
         <v>4</v>
@@ -4509,13 +4555,13 @@
         <v>3</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E3" s="12" t="s">
         <v>30</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G3" s="9" t="s">
         <v>7</v>
@@ -4532,10 +4578,10 @@
         <v>20</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E4" s="12" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="F4" s="9" t="s">
         <v>33</v>
@@ -4555,10 +4601,10 @@
         <v>40</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="F5" s="9" t="s">
         <v>49</v>
@@ -4578,10 +4624,10 @@
         <v>46</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="F6" s="9" t="s">
         <v>53</v>
@@ -4601,9 +4647,9 @@
         <v>59</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>140</v>
-      </c>
-      <c r="E7" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>61</v>
       </c>
       <c r="F7" s="9" t="s">
@@ -4624,9 +4670,9 @@
         <v>77</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="E8" s="9" t="s">
+        <v>139</v>
+      </c>
+      <c r="E8" s="12" t="s">
         <v>80</v>
       </c>
       <c r="F8" s="9" t="s">
@@ -4647,10 +4693,10 @@
         <v>86</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E9" s="12" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F9" s="9" t="s">
         <v>87</v>
@@ -4667,22 +4713,22 @@
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>103</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="D10" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="F10" s="9" t="s">
+      <c r="H10" s="9" t="s">
         <v>106</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>108</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>65</v>
@@ -4690,22 +4736,22 @@
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F11" s="9" t="s">
         <v>112</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="E11" s="12" t="s">
-        <v>160</v>
-      </c>
-      <c r="F11" s="9" t="s">
+      <c r="G11" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>114</v>
-      </c>
-      <c r="G11" s="9" t="s">
-        <v>115</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>116</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>65</v>
@@ -4713,22 +4759,22 @@
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
+        <v>115</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="D12" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F12" s="9" t="s">
+      <c r="H12" s="9" t="s">
         <v>118</v>
-      </c>
-      <c r="G12" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>120</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>65</v>
@@ -4736,22 +4782,22 @@
     </row>
     <row r="13" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
+        <v>122</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F13" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="H13" s="9" t="s">
         <v>124</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>146</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>164</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="G13" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>126</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>65</v>
@@ -4759,22 +4805,22 @@
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H14" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="J14" s="3" t="s">
         <v>65</v>
@@ -4785,51 +4831,77 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>3</v>
       </c>
       <c r="C16" s="9" t="s">
+        <v>294</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="G16" s="9" t="s">
         <v>296</v>
       </c>
-      <c r="E16" s="12" t="s">
-        <v>263</v>
-      </c>
-      <c r="F16" s="9" t="s">
+      <c r="H16" s="9" t="s">
         <v>297</v>
-      </c>
-      <c r="G16" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>299</v>
       </c>
       <c r="J16" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="E17" s="12" t="s">
         <v>309</v>
       </c>
-      <c r="C17" s="9" t="s">
+      <c r="F17" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="D17" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="E17" s="12" t="s">
+      <c r="G17" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="F17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>312</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>313</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>314</v>
+      <c r="J17" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B18" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="E18" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F18" s="9" t="s">
+        <v>324</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -4851,6 +4923,9 @@
     <hyperlink ref="E4" location="Sportorg_Sports!A1" display="sportorg/collections/sports"/>
     <hyperlink ref="E16" location="Sportorg_Games!A1" display="sportorg/models/game"/>
     <hyperlink ref="E17" location="Sportorg_TeamRosters!A1" display="sportorg/collections/teamrosters"/>
+    <hyperlink ref="E18" location="Media_Videos!A1" display="media/models/video"/>
+    <hyperlink ref="E7" location="User_Relateds!A1" display="user/collections/relateds"/>
+    <hyperlink ref="E8" location="User_FitnessBasics!A1" display="user/collections/fitnessbasics"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4858,10 +4933,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4875,24 +4950,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4963,227 +5038,324 @@
         <v>40</v>
       </c>
       <c r="E9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="26" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="26" t="s">
+        <v>300</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="6"/>
+    </row>
+    <row r="14" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="26" t="s">
+        <v>328</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="26" t="s">
+        <v>329</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="6"/>
+    </row>
+    <row r="16" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="26" t="s">
+        <v>330</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="26" t="s">
+        <v>331</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="6"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C19" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="6"/>
+    </row>
+    <row r="20" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C20" s="26" t="s">
+        <v>333</v>
+      </c>
+      <c r="E20" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="6"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>95</v>
+      </c>
+      <c r="E21" t="s">
+        <v>14</v>
+      </c>
+      <c r="F21" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="E24" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="E25" t="s">
         <v>101</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F25" s="6" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>94</v>
-      </c>
-      <c r="E10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>95</v>
-      </c>
-      <c r="E11" t="s">
-        <v>14</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>96</v>
-      </c>
-      <c r="E13" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>97</v>
-      </c>
-      <c r="E14" t="s">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="E26" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>98</v>
-      </c>
-      <c r="E15" t="s">
-        <v>101</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F26" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>99</v>
+      </c>
+      <c r="E27" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" t="s">
+      <c r="F27" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>100</v>
+      </c>
+      <c r="E28" t="s">
         <v>21</v>
       </c>
-      <c r="F17" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
-        <v>100</v>
-      </c>
-      <c r="E18" t="s">
-        <v>21</v>
-      </c>
-      <c r="F18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="F28" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B30" t="s">
         <v>11</v>
       </c>
-      <c r="E20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F20" s="7"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="E30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F30" s="7"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
         <v>26</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E33" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="F33" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>28</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E34" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="2" t="s">
+      <c r="F34" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="30"/>
-      <c r="E27" s="2" t="s">
+      <c r="B37" s="29" t="s">
+        <v>153</v>
+      </c>
+      <c r="C37" s="30"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F37" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G27" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F28"/>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F38"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>10</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E40" s="8"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>22</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B41" t="s">
         <v>11</v>
       </c>
-      <c r="E31" t="s">
-        <v>14</v>
-      </c>
-      <c r="F31" s="7"/>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+      <c r="E41" t="s">
+        <v>14</v>
+      </c>
+      <c r="F41" s="7"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
         <v>26</v>
       </c>
-      <c r="E34" t="s">
+      <c r="E44" t="s">
         <v>27</v>
       </c>
-      <c r="F34" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+      <c r="F44" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B45" t="s">
         <v>28</v>
       </c>
-      <c r="E35" t="s">
+      <c r="E45" t="s">
         <v>29</v>
       </c>
-      <c r="F35" s="6" t="b">
-        <v>0</v>
+      <c r="F45" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
+        <v>41359</v>
+      </c>
+      <c r="B48" t="s">
+        <v>327</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B37:D37"/>
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <hyperlinks>
@@ -5212,24 +5384,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>218</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5253,7 +5425,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E5" t="s">
         <v>21</v>
@@ -5264,7 +5436,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -5275,7 +5447,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -5338,11 +5510,11 @@
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="28" t="s">
-        <v>221</v>
-      </c>
-      <c r="C17" s="29"/>
-      <c r="D17" s="30"/>
+      <c r="B17" s="29" t="s">
+        <v>219</v>
+      </c>
+      <c r="C17" s="30"/>
+      <c r="D17" s="31"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -5354,12 +5526,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="31"/>
-      <c r="B18" s="31"/>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="31"/>
-      <c r="F18" s="31"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -5446,7 +5618,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5460,28 +5632,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5513,7 +5685,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E6" t="s">
         <v>21</v>
@@ -5593,7 +5765,7 @@
         <v>14</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -5628,7 +5800,7 @@
     </row>
     <row r="22" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -5636,7 +5808,7 @@
         <v>40984</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -5672,18 +5844,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>205</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5868,11 +6040,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="30"/>
+      <c r="B24" s="29" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="30"/>
+      <c r="D24" s="31"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -5966,18 +6138,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27"/>
-      <c r="B1" s="27"/>
+      <c r="A1" s="28"/>
+      <c r="B1" s="28"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>209</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>207</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6074,11 +6246,11 @@
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>210</v>
-      </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="30"/>
+      <c r="B15" s="29" t="s">
+        <v>208</v>
+      </c>
+      <c r="C15" s="30"/>
+      <c r="D15" s="31"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -6167,14 +6339,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6183,11 +6355,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>211</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>209</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6208,7 +6380,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
@@ -6219,7 +6391,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" t="s">
         <v>14</v>
@@ -6230,7 +6402,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" t="s">
         <v>14</v>
@@ -6241,7 +6413,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E7" t="s">
         <v>14</v>
@@ -6252,7 +6424,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E8" t="s">
         <v>14</v>
@@ -6263,7 +6435,7 @@
     </row>
     <row r="9" spans="1:7" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E9" s="15" t="s">
         <v>14</v>
@@ -6274,10 +6446,10 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>24</v>
@@ -6297,7 +6469,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6331,11 +6503,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>212</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>210</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6368,7 +6540,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6433,14 +6605,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6449,11 +6621,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>212</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6474,7 +6646,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -6485,7 +6657,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>14</v>
@@ -6496,7 +6668,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>14</v>
@@ -6507,7 +6679,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>14</v>
@@ -6518,7 +6690,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
@@ -6538,7 +6710,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6572,11 +6744,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>211</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6609,7 +6781,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6641,20 +6813,20 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="18" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>
@@ -6692,14 +6864,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6708,11 +6880,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>213</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6733,7 +6905,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -6744,7 +6916,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>14</v>
@@ -6755,7 +6927,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>14</v>
@@ -6766,7 +6938,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>14</v>
@@ -6786,7 +6958,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -6820,11 +6992,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>216</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>214</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6857,7 +7029,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -6922,14 +7094,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27" t="s">
-        <v>135</v>
-      </c>
-      <c r="D1" s="27"/>
+      <c r="A1" s="28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="28"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6938,11 +7110,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
-        <v>217</v>
-      </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="30"/>
+      <c r="B2" s="29" t="s">
+        <v>215</v>
+      </c>
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6963,7 +7135,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="15" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E4" s="15" t="s">
         <v>21</v>
@@ -6974,7 +7146,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E5" s="15" t="s">
         <v>14</v>
@@ -6985,7 +7157,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="15" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E6" s="15" t="s">
         <v>14</v>
@@ -6996,7 +7168,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>14</v>
@@ -7007,7 +7179,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
@@ -7027,7 +7199,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -7061,11 +7233,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="28" t="s">
-        <v>218</v>
-      </c>
-      <c r="C19" s="29"/>
-      <c r="D19" s="30"/>
+      <c r="B19" s="29" t="s">
+        <v>216</v>
+      </c>
+      <c r="C19" s="30"/>
+      <c r="D19" s="31"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7098,7 +7270,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Game Page - Video Thumbs, Image Grid, Fan Board
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="13" activeTab="19"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="366">
   <si>
     <t>User Profile</t>
   </si>
@@ -977,9 +977,6 @@
     <t>sportorg/collections/teamrosters</t>
   </si>
   <si>
-    <t>Team Rosters associated with the game</t>
-  </si>
-  <si>
     <t>api/game/teamrosters?game_id=101</t>
   </si>
   <si>
@@ -1047,6 +1044,105 @@
   </si>
   <si>
     <t>team2_name</t>
+  </si>
+  <si>
+    <t>videothumbs</t>
+  </si>
+  <si>
+    <t>game/collections/videothumbs</t>
+  </si>
+  <si>
+    <t>api/game/videothumbs?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/videothumbs/101</t>
+  </si>
+  <si>
+    <t>game/collections/images</t>
+  </si>
+  <si>
+    <t>Images associated with the game</t>
+  </si>
+  <si>
+    <t>api/game/images?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/images/101</t>
+  </si>
+  <si>
+    <t>addvideo</t>
+  </si>
+  <si>
+    <t>game/models/addvideo</t>
+  </si>
+  <si>
+    <t>Video information to add</t>
+  </si>
+  <si>
+    <t>api/game/addvideo?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/addvideo/101</t>
+  </si>
+  <si>
+    <t>addimage</t>
+  </si>
+  <si>
+    <t>game/models/addimage</t>
+  </si>
+  <si>
+    <t>Image information to add</t>
+  </si>
+  <si>
+    <t>api/game/addimage?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/addimage/101</t>
+  </si>
+  <si>
+    <t>game/collections/comments</t>
+  </si>
+  <si>
+    <t>List fo video thumbs associated with the game</t>
+  </si>
+  <si>
+    <t>List of team rosters associated with the game</t>
+  </si>
+  <si>
+    <t>List of comments associated with the game</t>
+  </si>
+  <si>
+    <t>api/game/comments?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/comments/101</t>
+  </si>
+  <si>
+    <t>commentform</t>
+  </si>
+  <si>
+    <t>game/modes/commentform</t>
+  </si>
+  <si>
+    <t>Leave a comment about the game</t>
+  </si>
+  <si>
+    <t>api/game/commentform?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/commentform/101</t>
+  </si>
+  <si>
+    <t>packages/media/models/videoservice</t>
+  </si>
+  <si>
+    <t>packages/media/collections/videoservices</t>
+  </si>
+  <si>
+    <t>service_id</t>
+  </si>
+  <si>
+    <t>website</t>
   </si>
 </sst>
 </file>
@@ -1208,7 +1304,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1259,6 +1355,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1588,7 +1685,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1606,10 +1703,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -1808,7 +1905,7 @@
         <v>307</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D18" s="9" t="s">
         <v>309</v>
@@ -1909,7 +2006,7 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="9" t="s">
+      <c r="B30" s="12" t="s">
         <v>160</v>
       </c>
       <c r="C30" s="9" t="s">
@@ -1944,6 +2041,7 @@
     <hyperlink ref="B13" location="Sportorg_Orgs!A1" display="orgs"/>
     <hyperlink ref="B12" location="Sportorg_Complevels!A1" display="complevels"/>
     <hyperlink ref="B18" location="Sportorg_TeamRosters!A1" display="teamrosters"/>
+    <hyperlink ref="B30" location="Media_VideoService!A1" display="videoservice"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1969,14 +2067,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -1985,11 +2083,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2108,11 +2206,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2211,14 +2309,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2227,11 +2325,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2350,11 +2448,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2453,14 +2551,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2469,11 +2567,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2603,11 +2701,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2706,14 +2804,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2722,11 +2820,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2834,11 +2932,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2943,14 +3041,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -2959,11 +3057,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3113,11 +3211,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3216,14 +3314,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3232,11 +3330,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3367,11 +3465,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3470,14 +3568,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -3486,11 +3584,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3638,11 +3736,11 @@
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="30" t="s">
         <v>256</v>
       </c>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="32"/>
       <c r="E22" s="2" t="s">
         <v>17</v>
       </c>
@@ -3769,14 +3867,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3785,11 +3883,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3928,11 +4026,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="30" t="s">
         <v>273</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4031,14 +4129,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4047,11 +4145,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="B2" s="30" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4072,7 +4170,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="23" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E4" s="23" t="s">
         <v>21</v>
@@ -4088,7 +4186,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" s="23" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E6" s="23" t="s">
         <v>38</v>
@@ -4104,7 +4202,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C8" s="23" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>14</v>
@@ -4120,7 +4218,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="23" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="E10" s="22" t="s">
         <v>14</v>
@@ -4145,7 +4243,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4179,11 +4277,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="29" t="s">
-        <v>320</v>
-      </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
+      <c r="B23" s="30" t="s">
+        <v>319</v>
+      </c>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4216,7 +4314,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4282,14 +4380,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4298,11 +4396,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4391,11 +4489,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="30" t="s">
         <v>285</v>
       </c>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="32"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4475,13 +4573,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4501,10 +4599,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="27"/>
+      <c r="B1" s="28"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -4855,13 +4953,10 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>307</v>
       </c>
-      <c r="C17" s="9" t="s">
-        <v>308</v>
-      </c>
       <c r="D17" s="9" t="s">
         <v>308</v>
       </c>
@@ -4869,39 +4964,186 @@
         <v>309</v>
       </c>
       <c r="F17" s="9" t="s">
+        <v>353</v>
+      </c>
+      <c r="G17" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="H17" s="9" t="s">
         <v>311</v>
-      </c>
-      <c r="H17" s="9" t="s">
-        <v>312</v>
       </c>
       <c r="J17" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>322</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>323</v>
       </c>
       <c r="E18" s="12" t="s">
         <v>158</v>
       </c>
       <c r="F18" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="G18" s="9" t="s">
         <v>324</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="H18" s="9" t="s">
         <v>325</v>
-      </c>
-      <c r="H18" s="9" t="s">
-        <v>326</v>
       </c>
       <c r="J18" s="3" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>334</v>
+      </c>
+      <c r="E19" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>335</v>
+      </c>
+      <c r="H19" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B20" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="H20" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
+        <v>341</v>
+      </c>
+      <c r="C21" s="9" t="s">
+        <v>342</v>
+      </c>
+      <c r="E21" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>343</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>344</v>
+      </c>
+      <c r="H21" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>347</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>348</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>349</v>
+      </c>
+      <c r="H22" s="9" t="s">
+        <v>350</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>355</v>
+      </c>
+      <c r="H23" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="E24" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>359</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="H24" s="9" t="s">
+        <v>361</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K24" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -4926,6 +5168,12 @@
     <hyperlink ref="E18" location="Media_Videos!A1" display="media/models/video"/>
     <hyperlink ref="E7" location="User_Relateds!A1" display="user/collections/relateds"/>
     <hyperlink ref="E8" location="User_FitnessBasics!A1" display="user/collections/fitnessbasics"/>
+    <hyperlink ref="E19" location="Media_Videos!A1" display="media/collections/videos"/>
+    <hyperlink ref="E20" location="Media_Images!A1" display="media/collections/images"/>
+    <hyperlink ref="E21" location="Media_Videos!A1" display="media/models/video"/>
+    <hyperlink ref="E22" location="Media_Images!A1" display="media/models/image"/>
+    <hyperlink ref="E23" location="Site_Comments!A1" display="site/collections/comments"/>
+    <hyperlink ref="E24" location="Site_Comments!A1" display="site/collections/comments"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4935,8 +5183,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4950,24 +5198,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5079,7 +5327,7 @@
     </row>
     <row r="14" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="26" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="E14" s="26" t="s">
         <v>36</v>
@@ -5088,7 +5336,7 @@
     </row>
     <row r="15" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D15" s="26" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="E15" s="26" t="s">
         <v>24</v>
@@ -5097,7 +5345,7 @@
     </row>
     <row r="16" spans="1:7" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D16" s="26" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="E16" s="26" t="s">
         <v>24</v>
@@ -5106,7 +5354,7 @@
     </row>
     <row r="17" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="D17" s="26" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E17" s="26" t="s">
         <v>24</v>
@@ -5123,7 +5371,7 @@
     </row>
     <row r="19" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C19" s="26" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E19" s="26" t="s">
         <v>14</v>
@@ -5132,7 +5380,7 @@
     </row>
     <row r="20" spans="1:6" s="26" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="26" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E20" s="26" t="s">
         <v>14</v>
@@ -5270,11 +5518,11 @@
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="29" t="s">
+      <c r="B37" s="30" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="32"/>
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
@@ -5348,7 +5596,7 @@
         <v>41359</v>
       </c>
       <c r="B48" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -5371,7 +5619,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5384,24 +5632,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5510,11 +5758,11 @@
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="30" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -5526,12 +5774,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="32"/>
-      <c r="C18" s="32"/>
-      <c r="D18" s="32"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -5602,12 +5850,222 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A27" sqref="A27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="27" customWidth="1"/>
+    <col min="2" max="2" width="15" style="27" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="27"/>
+    <col min="4" max="4" width="13.28515625" style="27" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="27" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="27" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="27"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>362</v>
+      </c>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F3" s="27"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="27" t="s">
+        <v>364</v>
+      </c>
+      <c r="E5" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="7"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" s="30" t="s">
+        <v>363</v>
+      </c>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="27"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="F20" s="7"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="F23" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="F24" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E27" s="6"/>
+      <c r="F27" s="27"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B16:D16"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Table of Contents"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages!A1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5632,14 +6090,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>204</v>
@@ -5649,11 +6107,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5844,18 +6302,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6040,11 +6498,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="30" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="32"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -6138,18 +6596,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28"/>
-      <c r="B1" s="28"/>
+      <c r="A1" s="29"/>
+      <c r="B1" s="29"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6246,11 +6704,11 @@
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="30" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="32"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -6339,14 +6797,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6355,11 +6813,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6503,11 +6961,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6605,14 +7063,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6621,11 +7079,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6744,11 +7202,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>211</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -6864,14 +7322,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6880,11 +7338,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6992,11 +7450,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7094,14 +7552,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28" t="s">
+      <c r="B1" s="29"/>
+      <c r="C1" s="29" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="28"/>
+      <c r="D1" s="29"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7110,11 +7568,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="30" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7233,11 +7691,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="30" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="30"/>
-      <c r="D19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
#6 clean html structure
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="8" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1286" uniqueCount="379">
   <si>
     <t>User Profile</t>
   </si>
@@ -1143,6 +1143,45 @@
   </si>
   <si>
     <t>website</t>
+  </si>
+  <si>
+    <t>Team</t>
+  </si>
+  <si>
+    <t>team/models/basics</t>
+  </si>
+  <si>
+    <t>Basic information about the team</t>
+  </si>
+  <si>
+    <t>api/team/basics?team_id=101</t>
+  </si>
+  <si>
+    <t>test/team/basics/101</t>
+  </si>
+  <si>
+    <t>change complevel to complevels</t>
+  </si>
+  <si>
+    <t>changed data type</t>
+  </si>
+  <si>
+    <t>change season to seasons</t>
+  </si>
+  <si>
+    <t>add sports, location, num_votes, num_followers</t>
+  </si>
+  <si>
+    <t>sport_id</t>
+  </si>
+  <si>
+    <t>complevel_id</t>
+  </si>
+  <si>
+    <t>complevel_name</t>
+  </si>
+  <si>
+    <t>season_id</t>
   </si>
 </sst>
 </file>
@@ -1304,7 +1343,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1355,6 +1394,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="5" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
@@ -1703,10 +1743,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -2067,14 +2107,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2083,11 +2123,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2206,11 +2246,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2309,14 +2349,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2325,11 +2365,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2448,11 +2488,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>223</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2551,14 +2591,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2567,11 +2607,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2701,11 +2741,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2804,14 +2844,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2820,11 +2860,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2932,11 +2972,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3041,14 +3081,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3057,11 +3097,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3211,11 +3251,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="31" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="33"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3295,10 +3335,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3314,14 +3354,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3330,11 +3370,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3372,124 +3412,145 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="E6" s="20" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="20" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="20" t="s">
-        <v>57</v>
-      </c>
-      <c r="E8" s="20" t="s">
+    <row r="6" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="28" t="s">
+        <v>252</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C8" s="28" t="s">
+        <v>375</v>
+      </c>
+      <c r="E8" s="28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="20" t="s">
-        <v>257</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>14</v>
-      </c>
+      <c r="F8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="20" t="s">
-        <v>258</v>
+        <v>291</v>
       </c>
       <c r="E10" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="20" t="s">
-        <v>259</v>
-      </c>
-      <c r="E11" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F14" s="7" t="s">
-        <v>45</v>
-      </c>
+    <row r="11" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="28" t="s">
+        <v>376</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="28" t="s">
+        <v>377</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="6"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" s="20" t="s">
+        <v>281</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="28" t="s">
+        <v>378</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="28" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
-        <v>25</v>
+      <c r="B16" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
-        <v>26</v>
+        <v>257</v>
       </c>
       <c r="E17" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F17" s="6">
-        <v>0</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B18" s="20" t="s">
-        <v>28</v>
+        <v>258</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="F18" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" s="30" t="s">
-        <v>256</v>
-      </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F21" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E22" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="E19" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E23" s="8"/>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="6"/>
+    </row>
+    <row r="22" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F22" s="6"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="20" t="s">
@@ -3502,7 +3563,7 @@
         <v>14</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>260</v>
+        <v>45</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -3530,6 +3591,106 @@
       </c>
       <c r="F28" s="6" t="b">
         <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B31" s="31" t="s">
+        <v>256</v>
+      </c>
+      <c r="C31" s="32"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F34" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E37" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F38" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="14">
+        <v>41362</v>
+      </c>
+      <c r="B41" s="20" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="20" t="s">
+        <v>371</v>
+      </c>
+      <c r="E42" s="20" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="20" t="s">
+        <v>373</v>
+      </c>
+      <c r="E43" s="20" t="s">
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -3537,7 +3698,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B31:D31"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
@@ -3552,7 +3713,7 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3568,14 +3729,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -3584,11 +3745,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3736,11 +3897,11 @@
       <c r="A22" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="31" t="s">
         <v>256</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="32"/>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
       <c r="E22" s="2" t="s">
         <v>17</v>
       </c>
@@ -3867,14 +4028,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3883,11 +4044,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4026,11 +4187,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>273</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4129,14 +4290,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4145,11 +4306,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>314</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4277,11 +4438,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>319</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4380,14 +4541,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4396,11 +4557,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4489,11 +4650,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="31" t="s">
         <v>285</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="32"/>
+      <c r="C23" s="32"/>
+      <c r="D23" s="33"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4573,13 +4734,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L24"/>
+  <dimension ref="A1:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C9" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4599,10 +4760,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="28"/>
+      <c r="B1" s="29"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -4953,7 +5114,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>307</v>
       </c>
@@ -4976,7 +5137,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
         <v>321</v>
       </c>
@@ -4999,7 +5160,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B19" s="9" t="s">
         <v>333</v>
       </c>
@@ -5022,7 +5183,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B20" s="9" t="s">
         <v>103</v>
       </c>
@@ -5045,7 +5206,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
         <v>341</v>
       </c>
@@ -5071,7 +5232,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
         <v>346</v>
       </c>
@@ -5097,7 +5258,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
         <v>164</v>
       </c>
@@ -5120,7 +5281,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
         <v>357</v>
       </c>
@@ -5144,6 +5305,32 @@
       </c>
       <c r="K24" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>367</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>368</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>369</v>
+      </c>
+      <c r="H26" s="9" t="s">
+        <v>370</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
@@ -5174,6 +5361,7 @@
     <hyperlink ref="E22" location="Media_Images!A1" display="media/models/image"/>
     <hyperlink ref="E23" location="Site_Comments!A1" display="site/collections/comments"/>
     <hyperlink ref="E24" location="Site_Comments!A1" display="site/collections/comments"/>
+    <hyperlink ref="E26" location="Sportorg_Teams!A1" display="sportorg/models/team"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5198,24 +5386,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5518,11 +5706,11 @@
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="31" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="32"/>
+      <c r="C37" s="32"/>
+      <c r="D37" s="33"/>
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
@@ -5632,24 +5820,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5758,11 +5946,11 @@
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="31" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="32"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -5774,12 +5962,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="33"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="33"/>
+      <c r="A18" s="34"/>
+      <c r="B18" s="34"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -5869,24 +6057,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>362</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5978,11 +6166,11 @@
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="31" t="s">
         <v>363</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
@@ -6090,14 +6278,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>204</v>
@@ -6107,11 +6295,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6302,18 +6490,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6498,11 +6686,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="32"/>
+      <c r="C24" s="32"/>
+      <c r="D24" s="33"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -6596,18 +6784,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29"/>
-      <c r="B1" s="29"/>
+      <c r="A1" s="30"/>
+      <c r="B1" s="30"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6704,11 +6892,11 @@
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -6797,14 +6985,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -6813,11 +7001,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6961,11 +7149,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7063,14 +7251,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7079,11 +7267,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7202,11 +7390,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>211</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7322,14 +7510,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7338,11 +7526,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7450,11 +7638,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7552,14 +7740,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="30"/>
+      <c r="C1" s="30" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="29"/>
+      <c r="D1" s="30"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7568,11 +7756,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="31" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7691,11 +7879,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="31" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="32"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
add content buttons and schedule - team page
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="14" activeTab="18"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="9" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="411">
   <si>
     <t>User Profile</t>
   </si>
@@ -1235,10 +1235,55 @@
     <t xml:space="preserve">List of seasons associated with team, sport and complevel </t>
   </si>
   <si>
-    <t>api/team/seasons?team_id=101&amp;sport_id=1&amp;season_id=1</t>
-  </si>
-  <si>
     <t>test/team/seasons/101/1/1</t>
+  </si>
+  <si>
+    <t>points_against</t>
+  </si>
+  <si>
+    <t>is_winner</t>
+  </si>
+  <si>
+    <t>upcoming_schedules</t>
+  </si>
+  <si>
+    <t>team/collections/upcoming_schedules</t>
+  </si>
+  <si>
+    <t>recent_schedules</t>
+  </si>
+  <si>
+    <t>team/collections/recent_schedules</t>
+  </si>
+  <si>
+    <t>api/team/seasons?team_id=101&amp;sport_id=1&amp;complevel_id=1</t>
+  </si>
+  <si>
+    <t>List of upcoming schedules associated with team, sport 
+and complevel, season</t>
+  </si>
+  <si>
+    <t>List of recent schedules associated with team, sport 
+and complevel, season</t>
+  </si>
+  <si>
+    <t>api/team/upcoming_schedules?team_id=101&amp;sport_id=1
+&amp;complevel_id=1&amp;season_id=1</t>
+  </si>
+  <si>
+    <t>test/team/upcoming_schedules/
+101/1/1/1</t>
+  </si>
+  <si>
+    <t>api/team/recent_schedules?team_id=101&amp;sport_id=1
+&amp;complevel_id=1&amp;season_id=1</t>
+  </si>
+  <si>
+    <t>test/team/recent_schedules/
+101/1/1/1</t>
+  </si>
+  <si>
+    <t>W or L</t>
   </si>
 </sst>
 </file>
@@ -1407,7 +1452,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1462,6 +1507,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1478,15 +1533,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -1799,7 +1845,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
+      <selection pane="bottomRight" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1817,10 +1863,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -2181,14 +2227,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2197,11 +2243,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2320,11 +2366,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2423,14 +2469,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2439,11 +2485,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2593,11 +2639,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="38" t="s">
         <v>223</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2709,14 +2755,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2725,11 +2771,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2859,11 +2905,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2962,14 +3008,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2978,11 +3024,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3090,11 +3136,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3199,14 +3245,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3215,11 +3261,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3369,11 +3415,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="38" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="33"/>
-      <c r="D21" s="34"/>
+      <c r="C21" s="39"/>
+      <c r="D21" s="40"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3472,14 +3518,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3488,11 +3534,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3548,86 +3594,86 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="36" t="s">
+    <row r="8" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="F8" s="37"/>
-    </row>
-    <row r="9" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="36" t="s">
+      <c r="F8" s="32"/>
+    </row>
+    <row r="9" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C9" s="31" t="s">
         <v>375</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="37"/>
-    </row>
-    <row r="10" spans="1:7" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="36" t="s">
+      <c r="F9" s="32"/>
+    </row>
+    <row r="10" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C10" s="31" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="36" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="37"/>
-    </row>
-    <row r="11" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="39" t="s">
+      <c r="E10" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="F10" s="32"/>
+    </row>
+    <row r="11" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="34" t="s">
         <v>291</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="F11" s="40"/>
-    </row>
-    <row r="12" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="39" t="s">
+      <c r="F11" s="35"/>
+    </row>
+    <row r="12" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="34" t="s">
         <v>376</v>
       </c>
-      <c r="E12" s="39" t="s">
+      <c r="E12" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="40"/>
-    </row>
-    <row r="13" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="39" t="s">
+      <c r="F12" s="35"/>
+    </row>
+    <row r="13" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C13" s="34" t="s">
         <v>377</v>
       </c>
-      <c r="E13" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="40"/>
-    </row>
-    <row r="14" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="39" t="s">
+      <c r="E13" s="34" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="35"/>
+    </row>
+    <row r="14" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="34" t="s">
         <v>281</v>
       </c>
-      <c r="E14" s="38" t="s">
+      <c r="E14" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="F14" s="40"/>
-    </row>
-    <row r="15" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="39" t="s">
+      <c r="F14" s="35"/>
+    </row>
+    <row r="15" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="34" t="s">
         <v>378</v>
       </c>
-      <c r="E15" s="38" t="s">
+      <c r="E15" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="40"/>
-    </row>
-    <row r="16" spans="1:7" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="39" t="s">
+      <c r="F15" s="35"/>
+    </row>
+    <row r="16" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="34" t="s">
         <v>287</v>
       </c>
-      <c r="E16" s="38" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="40"/>
+      <c r="E16" s="33" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="35"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B17" s="20" t="s">
@@ -3726,11 +3772,11 @@
       <c r="A32" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="C32" s="33"/>
-      <c r="D32" s="34"/>
+      <c r="C32" s="39"/>
+      <c r="D32" s="40"/>
       <c r="E32" s="2" t="s">
         <v>17</v>
       </c>
@@ -3847,10 +3893,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3866,14 +3912,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -3882,11 +3928,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3973,159 +4019,179 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="20" t="s">
+    <row r="12" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="30" t="s">
         <v>302</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="30" t="s">
         <v>21</v>
       </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="20" t="s">
+      <c r="C13" s="20" t="s">
+        <v>397</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C14" s="30" t="s">
+        <v>398</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
         <v>303</v>
       </c>
-      <c r="E13" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" s="20" t="s">
-        <v>11</v>
-      </c>
       <c r="E15" s="20" t="s">
         <v>14</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F18" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E21" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="2" t="s">
+      <c r="F21" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B24" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="C22" s="33"/>
-      <c r="D22" s="34"/>
-      <c r="E22" s="2" t="s">
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F22" s="5" t="s">
+      <c r="F24" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G22" s="2" t="s">
+      <c r="G24" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E24" s="8"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="E25" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="7" t="s">
-        <v>268</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="8"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E30" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="F30" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E31" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="24" t="s">
+      <c r="F31" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="F32" s="25"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+      <c r="F34" s="25"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="14">
         <v>41352</v>
       </c>
-      <c r="B33" s="20" t="s">
+      <c r="B35" s="20" t="s">
         <v>306</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C35" s="20" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="14">
         <v>41353</v>
       </c>
-      <c r="B34" s="21" t="s">
+      <c r="B36" s="21" t="s">
         <v>306</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C36" s="20" t="s">
         <v>305</v>
       </c>
     </row>
@@ -4134,7 +4200,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B24:D24"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
@@ -4149,7 +4215,7 @@
   <dimension ref="A1:G30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4165,14 +4231,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4181,11 +4247,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4324,11 +4390,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="38" t="s">
         <v>273</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4427,14 +4493,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4443,11 +4509,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>314</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4575,11 +4641,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="38" t="s">
         <v>319</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4661,8 +4727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4678,14 +4744,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4694,11 +4760,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>284</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4787,11 +4853,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="38" t="s">
         <v>285</v>
       </c>
-      <c r="C23" s="33"/>
-      <c r="D23" s="34"/>
+      <c r="C23" s="39"/>
+      <c r="D23" s="40"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4871,21 +4937,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E29" sqref="E29"/>
+      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="9" customWidth="1"/>
-    <col min="2" max="2" width="16" style="9" customWidth="1"/>
-    <col min="3" max="3" width="31.85546875" style="9" customWidth="1"/>
-    <col min="4" max="5" width="33.28515625" style="9" customWidth="1"/>
+    <col min="2" max="2" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.28515625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="36.28515625" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="9" customWidth="1"/>
     <col min="6" max="7" width="53.7109375" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="30.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="7.85546875" style="3" customWidth="1"/>
@@ -4896,10 +4963,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="30"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -5529,12 +5596,58 @@
         <v>395</v>
       </c>
       <c r="G29" s="9" t="s">
+        <v>403</v>
+      </c>
+      <c r="H29" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="H29" s="9" t="s">
-        <v>397</v>
-      </c>
       <c r="J29" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="9" t="s">
+        <v>399</v>
+      </c>
+      <c r="D30" s="9" t="s">
+        <v>400</v>
+      </c>
+      <c r="E30" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F30" s="13" t="s">
+        <v>404</v>
+      </c>
+      <c r="G30" s="13" t="s">
+        <v>406</v>
+      </c>
+      <c r="H30" s="13" t="s">
+        <v>407</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B31" s="9" t="s">
+        <v>401</v>
+      </c>
+      <c r="D31" s="9" t="s">
+        <v>402</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>405</v>
+      </c>
+      <c r="G31" s="13" t="s">
+        <v>408</v>
+      </c>
+      <c r="H31" s="13" t="s">
+        <v>409</v>
+      </c>
+      <c r="J31" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5570,6 +5683,8 @@
     <hyperlink ref="E27" location="Sportorg_Sports!A1" display="sportorg/collections/sports"/>
     <hyperlink ref="E28" location="Sportorg_Complevels!A1" display="sportorg/collections/complevels"/>
     <hyperlink ref="E29" location="Sportorg_Seasons!A1" display="sportorg/collections/seasons"/>
+    <hyperlink ref="E30" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
+    <hyperlink ref="E31" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5594,24 +5709,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5914,11 +6029,11 @@
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="32" t="s">
+      <c r="B37" s="38" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="33"/>
-      <c r="D37" s="34"/>
+      <c r="C37" s="39"/>
+      <c r="D37" s="40"/>
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
@@ -6028,24 +6143,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6154,11 +6269,11 @@
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="38" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="34"/>
+      <c r="C17" s="39"/>
+      <c r="D17" s="40"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -6170,12 +6285,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
+      <c r="A18" s="41"/>
+      <c r="B18" s="41"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -6265,24 +6380,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>362</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6374,11 +6489,11 @@
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="38" t="s">
         <v>363</v>
       </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="34"/>
+      <c r="C16" s="39"/>
+      <c r="D16" s="40"/>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
@@ -6486,14 +6601,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>204</v>
@@ -6503,11 +6618,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6698,18 +6813,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6894,11 +7009,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="38" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="33"/>
-      <c r="D24" s="34"/>
+      <c r="C24" s="39"/>
+      <c r="D24" s="40"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -6992,18 +7107,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31"/>
-      <c r="B1" s="31"/>
+      <c r="A1" s="37"/>
+      <c r="B1" s="37"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7100,11 +7215,11 @@
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="38" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="33"/>
-      <c r="D15" s="34"/>
+      <c r="C15" s="39"/>
+      <c r="D15" s="40"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -7193,14 +7308,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7209,11 +7324,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7357,11 +7472,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7459,14 +7574,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7475,11 +7590,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7598,11 +7713,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>211</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7718,14 +7833,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7734,11 +7849,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7846,11 +7961,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7948,14 +8063,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="37" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="31"/>
+      <c r="D1" s="37"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7964,11 +8079,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="38" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="34"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8087,11 +8202,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="38" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="33"/>
-      <c r="D19" s="34"/>
+      <c r="C19" s="39"/>
+      <c r="D19" s="40"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
#325 Competitor Teams List - Team Page
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="9" activeTab="15"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="417">
   <si>
     <t>User Profile</t>
   </si>
@@ -1284,13 +1284,34 @@
   </si>
   <si>
     <t>W or L</t>
+  </si>
+  <si>
+    <t>add sport, complevel, season</t>
+  </si>
+  <si>
+    <t>competitor_teams</t>
+  </si>
+  <si>
+    <t>team/collections/competitor_teams</t>
+  </si>
+  <si>
+    <t>List of competitor teams associated with team, sport 
+and complevel, season</t>
+  </si>
+  <si>
+    <t>api/team/competitor_teams?team_id=101&amp;sport_id=1
+&amp;complevel_id=1&amp;season_id=1</t>
+  </si>
+  <si>
+    <t>test/team/competitor_teams/
+101/1/1/1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1346,6 +1367,12 @@
     <font>
       <sz val="11"/>
       <color theme="0" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1452,7 +1479,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1533,6 +1560,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -1845,7 +1874,7 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:B1"/>
+      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3499,7 +3528,7 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G45"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1:D1"/>
@@ -3675,205 +3704,246 @@
       </c>
       <c r="F16" s="35"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="20" t="s">
+    <row r="17" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="42" t="s">
+        <v>73</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="35"/>
+    </row>
+    <row r="18" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F18" s="35"/>
+    </row>
+    <row r="19" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42"/>
+      <c r="E19" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="F19" s="35"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E20" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="20" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
         <v>257</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+      <c r="E21" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
         <v>258</v>
       </c>
-      <c r="E19" s="20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="E22" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="20" t="s">
         <v>259</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E23" s="20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="20" t="s">
+      <c r="E24" s="20" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="28" t="s">
+    <row r="25" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E22" s="28" t="s">
+      <c r="E25" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F23" s="6"/>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="F25" s="6"/>
+    </row>
+    <row r="26" spans="1:6" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F26" s="6"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B28" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="7" t="s">
+      <c r="E28" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="20" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="20" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E28" s="20" t="s">
+      <c r="E31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="F31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E32" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="2" t="s">
+      <c r="F32" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B35" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="C32" s="39"/>
-      <c r="D32" s="40"/>
-      <c r="E32" s="2" t="s">
+      <c r="C35" s="39"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="F32" s="5" t="s">
+      <c r="F35" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="G32" s="2" t="s">
+      <c r="G35" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="20" t="s">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="B38" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="E35" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="F35" s="7" t="s">
+      <c r="E38" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F38" s="7" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="20" t="s">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" s="20" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B38" s="20" t="s">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B41" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="E38" s="20" t="s">
+      <c r="E41" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="20" t="s">
+      <c r="F41" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B42" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E39" s="20" t="s">
+      <c r="E42" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F39" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="18" t="s">
+      <c r="F42" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="18" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="14">
         <v>41362</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B45" s="20" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="20" t="s">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B46" s="20" t="s">
         <v>371</v>
       </c>
-      <c r="E43" s="20" t="s">
+      <c r="E46" s="20" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B44" s="20" t="s">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B47" s="20" t="s">
         <v>373</v>
       </c>
-      <c r="E44" s="20" t="s">
+      <c r="E47" s="20" t="s">
         <v>372</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="14">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="14">
         <v>41367</v>
       </c>
-      <c r="B45" s="20" t="s">
+      <c r="B48" s="20" t="s">
         <v>387</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="14">
+        <v>41369</v>
+      </c>
+      <c r="B49" s="20" t="s">
+        <v>411</v>
       </c>
     </row>
   </sheetData>
@@ -3881,7 +3951,7 @@
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="C1:D1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B35:D35"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
@@ -3895,8 +3965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4937,13 +5007,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C21" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E30" sqref="E30"/>
+      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5648,6 +5718,29 @@
         <v>409</v>
       </c>
       <c r="J31" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="B32" s="9" t="s">
+        <v>412</v>
+      </c>
+      <c r="D32" s="9" t="s">
+        <v>413</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>254</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>414</v>
+      </c>
+      <c r="G32" s="13" t="s">
+        <v>415</v>
+      </c>
+      <c r="H32" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="J32" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5685,6 +5778,7 @@
     <hyperlink ref="E29" location="Sportorg_Seasons!A1" display="sportorg/collections/seasons"/>
     <hyperlink ref="E30" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
     <hyperlink ref="E31" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
+    <hyperlink ref="E32" location="Sportorg_Teams!A1" display="sportorg/collections/teams"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
#331 Rosters - Team Page
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -24,18 +24,19 @@
     <sheet name="Sportorg_Teams" sheetId="24" r:id="rId15"/>
     <sheet name="Sportorg_Games" sheetId="25" r:id="rId16"/>
     <sheet name="Sportorg_Matches" sheetId="26" r:id="rId17"/>
-    <sheet name="Sportorg_TeamRosters" sheetId="28" r:id="rId18"/>
-    <sheet name="Sportorg_Seasons" sheetId="27" r:id="rId19"/>
-    <sheet name="Media_Videos" sheetId="8" r:id="rId20"/>
-    <sheet name="Media_Images" sheetId="9" r:id="rId21"/>
-    <sheet name="Media_VideoService" sheetId="19" r:id="rId22"/>
+    <sheet name="Sportorg_Rosters" sheetId="29" r:id="rId18"/>
+    <sheet name="Sportorg_TeamRosters" sheetId="28" r:id="rId19"/>
+    <sheet name="Sportorg_Seasons" sheetId="27" r:id="rId20"/>
+    <sheet name="Media_Videos" sheetId="8" r:id="rId21"/>
+    <sheet name="Media_Images" sheetId="9" r:id="rId22"/>
+    <sheet name="Media_VideoService" sheetId="19" r:id="rId23"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1352" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="427">
   <si>
     <t>User Profile</t>
   </si>
@@ -1305,6 +1306,38 @@
   <si>
     <t>test/team/competitor_teams/
 101/1/1/1</t>
+  </si>
+  <si>
+    <t>api/team/teamrosters?team_id=101&amp;sport_id=1
+&amp;complevel_id=1&amp;season_id=1</t>
+  </si>
+  <si>
+    <t>test/team/teamrosters/101/1/1/1</t>
+  </si>
+  <si>
+    <t>sportorg/collections/rosters</t>
+  </si>
+  <si>
+    <t>sportorg/models/roster</t>
+  </si>
+  <si>
+    <t>packages/sportorg/models/roster</t>
+  </si>
+  <si>
+    <t>packages/sportorg/collections/rosters</t>
+  </si>
+  <si>
+    <t>List of rosters</t>
+  </si>
+  <si>
+    <t>Roster information</t>
+  </si>
+  <si>
+    <t>List of rosters associated with team, sport 
+and complevel, season</t>
+  </si>
+  <si>
+    <t>team/collections/rosters</t>
   </si>
 </sst>
 </file>
@@ -1479,7 +1512,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1544,6 +1577,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1560,8 +1596,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -1868,13 +1902,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1892,10 +1926,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -2101,104 +2135,115 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="17"/>
+      <c r="B19" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>420</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>419</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B20" s="17"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B21" s="17" t="s">
+      <c r="B22" s="17" t="s">
         <v>164</v>
       </c>
-      <c r="C21" s="9" t="s">
+      <c r="C22" s="9" t="s">
         <v>165</v>
       </c>
-      <c r="D21" s="9" t="s">
+      <c r="D22" s="9" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="17" t="s">
-        <v>174</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>175</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="13"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="17" t="s">
-        <v>98</v>
+        <v>174</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
-        <v>190</v>
+        <v>98</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>192</v>
-      </c>
+        <v>186</v>
+      </c>
+      <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
+        <v>190</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="9" t="s">
+      <c r="C26" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="D25" s="9" t="s">
+      <c r="D26" s="9" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="17"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="17"/>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B28" s="17" t="s">
+      <c r="B29" s="17" t="s">
         <v>86</v>
       </c>
-      <c r="C28" s="9" t="s">
+      <c r="C29" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="D28" s="9" t="s">
+      <c r="D29" s="9" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" s="17" t="s">
         <v>103</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="12" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="12" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>161</v>
       </c>
     </row>
@@ -2215,11 +2260,11 @@
     <hyperlink ref="B6" location="User_Orgs!A1" display="orgs"/>
     <hyperlink ref="B7" location="User_Relateds!A1" display="relateds"/>
     <hyperlink ref="B8" location="User_FitnessBasics!A1" display="fitnessbasics"/>
-    <hyperlink ref="B21" location="Site_Comments!A1" display="comments"/>
-    <hyperlink ref="B28" location="Media_Videos!A1" display="videos"/>
-    <hyperlink ref="B29" location="Media_Images!A1" display="images"/>
-    <hyperlink ref="B22" location="Site_Pogs!A1" display="pogs"/>
-    <hyperlink ref="B23" location="Site_Tags!A1" display="tags"/>
+    <hyperlink ref="B22" location="Site_Comments!A1" display="comments"/>
+    <hyperlink ref="B29" location="Media_Videos!A1" display="videos"/>
+    <hyperlink ref="B30" location="Media_Images!A1" display="images"/>
+    <hyperlink ref="B23" location="Site_Pogs!A1" display="pogs"/>
+    <hyperlink ref="B24" location="Site_Tags!A1" display="tags"/>
     <hyperlink ref="B10" location="Sportorg_Sports!A1" display="sports"/>
     <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
     <hyperlink ref="B11" location="Sportorg_Positions!A1" display="positions"/>
@@ -2230,7 +2275,8 @@
     <hyperlink ref="B13" location="Sportorg_Orgs!A1" display="orgs"/>
     <hyperlink ref="B12" location="Sportorg_Complevels!A1" display="complevels"/>
     <hyperlink ref="B18" location="Sportorg_TeamRosters!A1" display="teamrosters"/>
-    <hyperlink ref="B30" location="Media_VideoService!A1" display="videoservice"/>
+    <hyperlink ref="B31" location="Media_VideoService!A1" display="videoservice"/>
+    <hyperlink ref="B19" location="Sportorg_Rosters!A1" display="rosters"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2256,14 +2302,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2272,11 +2318,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2395,11 +2441,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2498,14 +2544,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2514,11 +2560,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>222</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2668,11 +2714,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2784,14 +2830,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2800,11 +2846,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>231</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2934,11 +2980,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>234</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3037,14 +3083,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -3053,11 +3099,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>239</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3165,11 +3211,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>289</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3274,14 +3320,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3290,11 +3336,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>245</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3444,11 +3490,11 @@
       <c r="A21" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="41" t="s">
         <v>246</v>
       </c>
-      <c r="C21" s="39"/>
-      <c r="D21" s="40"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="43"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3547,14 +3593,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3563,11 +3609,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3705,34 +3751,34 @@
       <c r="F16" s="35"/>
     </row>
     <row r="17" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="42" t="s">
+      <c r="B17" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="43" t="s">
+      <c r="C17" s="37"/>
+      <c r="D17" s="37"/>
+      <c r="E17" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="35"/>
     </row>
     <row r="18" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="42" t="s">
+      <c r="B18" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="43" t="s">
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="35"/>
     </row>
     <row r="19" spans="1:6" s="34" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="43" t="s">
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38" t="s">
         <v>14</v>
       </c>
       <c r="F19" s="35"/>
@@ -3834,11 +3880,11 @@
       <c r="A35" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="41" t="s">
         <v>256</v>
       </c>
-      <c r="C35" s="39"/>
-      <c r="D35" s="40"/>
+      <c r="C35" s="42"/>
+      <c r="D35" s="43"/>
       <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
@@ -3982,14 +4028,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -3998,11 +4044,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>263</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4170,11 +4216,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="41" t="s">
         <v>256</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4301,14 +4347,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4317,11 +4363,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>272</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4460,11 +4506,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="41" t="s">
         <v>273</v>
       </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4552,25 +4598,25 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="23" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="23" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="36" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="36" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="36" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="36" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="36" customWidth="1"/>
     <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" style="23" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="23"/>
+    <col min="7" max="7" width="62.28515625" style="36" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4579,11 +4625,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>314</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="41" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4595,7 +4641,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -4603,93 +4649,85 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>315</v>
-      </c>
-      <c r="E4" s="23" t="s">
+      <c r="B4" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="36" t="s">
+        <v>317</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="36" t="s">
+        <v>129</v>
+      </c>
+      <c r="E6" s="22" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>300</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>316</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="23" t="s">
-        <v>58</v>
+      <c r="B7" s="36" t="s">
+        <v>318</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="23" t="s">
-        <v>317</v>
+      <c r="B8" s="36" t="s">
+        <v>37</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="23" t="s">
-        <v>129</v>
+      <c r="B9" s="36" t="s">
+        <v>19</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="23" t="s">
-        <v>318</v>
+      <c r="B10" s="36" t="s">
+        <v>72</v>
       </c>
       <c r="E10" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="23" t="s">
+      <c r="E16" s="36" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>313</v>
+        <v>424</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="36" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
+      <c r="B19" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="23" t="s">
+      <c r="E19" s="36" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="6">
@@ -4697,10 +4735,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="23" t="s">
+      <c r="E20" s="36" t="s">
         <v>29</v>
       </c>
       <c r="F20" s="6" t="b">
@@ -4711,11 +4749,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
+      <c r="B23" s="41" t="s">
+        <v>422</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4727,7 +4765,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
+      <c r="A24" s="36" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -4738,29 +4776,29 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
+      <c r="A26" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="36" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>312</v>
+        <v>423</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
+      <c r="A28" s="36" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
+      <c r="B29" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="36" t="s">
         <v>27</v>
       </c>
       <c r="F29" s="6">
@@ -4768,10 +4806,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="36" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="6" t="b">
@@ -4797,31 +4835,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="17" style="20" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="20"/>
-    <col min="4" max="4" width="12.7109375" style="20" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="23" customWidth="1"/>
     <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" style="20" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="20"/>
+    <col min="7" max="7" width="62.28515625" style="23" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="23"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4830,11 +4868,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
-        <v>284</v>
-      </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="41" t="s">
+        <v>314</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4846,7 +4884,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="A3" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
@@ -4854,54 +4892,93 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="20" t="s">
-        <v>378</v>
-      </c>
-      <c r="E4" s="20" t="s">
+      <c r="B4" s="23" t="s">
+        <v>315</v>
+      </c>
+      <c r="E4" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="20" t="s">
-        <v>287</v>
-      </c>
-      <c r="E5" s="20" t="s">
-        <v>14</v>
+      <c r="B5" s="23" t="s">
+        <v>300</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>316</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E7" s="22"/>
+      <c r="C7" s="23" t="s">
+        <v>58</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="22"/>
+      <c r="C8" s="23" t="s">
+        <v>317</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="22"/>
+      <c r="C9" s="23" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="23" t="s">
+        <v>318</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>286</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="20" t="s">
+      <c r="A18" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="23" t="s">
         <v>27</v>
       </c>
       <c r="F19" s="6">
@@ -4909,10 +4986,10 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="20" t="s">
+      <c r="B20" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E20" s="20" t="s">
+      <c r="E20" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F20" s="6" t="b">
@@ -4923,11 +5000,11 @@
       <c r="A23" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B23" s="38" t="s">
-        <v>285</v>
-      </c>
-      <c r="C23" s="39"/>
-      <c r="D23" s="40"/>
+      <c r="B23" s="41" t="s">
+        <v>319</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4939,7 +5016,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="20" t="s">
+      <c r="A24" s="23" t="s">
         <v>10</v>
       </c>
       <c r="E24" s="1" t="s">
@@ -4950,29 +5027,29 @@
       <c r="E25" s="8"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="20" t="s">
+      <c r="A26" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="20" t="s">
+      <c r="B26" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="E26" s="20" t="s">
+      <c r="E26" s="23" t="s">
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="20" t="s">
+      <c r="A28" s="23" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="23" t="s">
         <v>26</v>
       </c>
-      <c r="E29" s="20" t="s">
+      <c r="E29" s="23" t="s">
         <v>27</v>
       </c>
       <c r="F29" s="6">
@@ -4980,10 +5057,10 @@
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="6" t="b">
@@ -5007,13 +5084,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="H33" sqref="H33"/>
+      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5033,10 +5110,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="36"/>
+      <c r="B1" s="39"/>
       <c r="C1" s="16" t="s">
         <v>133</v>
       </c>
@@ -5741,6 +5818,29 @@
         <v>416</v>
       </c>
       <c r="J32" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>316</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>426</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>425</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>417</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="J33" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5779,12 +5879,225 @@
     <hyperlink ref="E30" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
     <hyperlink ref="E31" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
     <hyperlink ref="E32" location="Sportorg_Teams!A1" display="sportorg/collections/teams"/>
+    <hyperlink ref="E33" location="Sportorg_Rosters!A1" display="sportorg/collections/rosters"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="20" customWidth="1"/>
+    <col min="2" max="2" width="17" style="20" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="20"/>
+    <col min="4" max="4" width="12.7109375" style="20" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="20" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="20" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="20"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="40" t="s">
+        <v>132</v>
+      </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="40"/>
+      <c r="E1" s="14">
+        <v>41352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>284</v>
+      </c>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="20" t="s">
+        <v>378</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
+        <v>287</v>
+      </c>
+      <c r="E5" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E7" s="22"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="22"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E9" s="22"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="C23" s="42"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B23:D23"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
@@ -5803,24 +6116,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>152</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6123,11 +6436,11 @@
       <c r="A37" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="C37" s="39"/>
-      <c r="D37" s="40"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="43"/>
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
@@ -6219,7 +6532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -6237,24 +6550,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6363,11 +6676,11 @@
       <c r="A17" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="C17" s="39"/>
-      <c r="D17" s="40"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="43"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -6379,12 +6692,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="41"/>
-      <c r="B18" s="41"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="A18" s="44"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -6453,7 +6766,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -6474,24 +6787,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>362</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6583,11 +6896,11 @@
       <c r="A16" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="41" t="s">
         <v>363</v>
       </c>
-      <c r="C16" s="39"/>
-      <c r="D16" s="40"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="43"/>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
@@ -6695,14 +7008,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>204</v>
@@ -6712,11 +7025,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6907,18 +7220,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>205</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7103,11 +7416,11 @@
       <c r="A24" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="41" t="s">
         <v>206</v>
       </c>
-      <c r="C24" s="39"/>
-      <c r="D24" s="40"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="43"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -7201,18 +7514,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37"/>
-      <c r="B1" s="37"/>
+      <c r="A1" s="40"/>
+      <c r="B1" s="40"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7309,11 +7622,11 @@
       <c r="A15" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="41" t="s">
         <v>208</v>
       </c>
-      <c r="C15" s="39"/>
-      <c r="D15" s="40"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="43"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -7402,14 +7715,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7418,11 +7731,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>209</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7566,11 +7879,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>210</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7668,14 +7981,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7684,11 +7997,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7807,11 +8120,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -7927,14 +8240,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7943,11 +8256,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8055,11 +8368,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -8157,14 +8470,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="40" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37" t="s">
+      <c r="B1" s="40"/>
+      <c r="C1" s="40" t="s">
         <v>133</v>
       </c>
-      <c r="D1" s="37"/>
+      <c r="D1" s="40"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -8173,11 +8486,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="41" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="40"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="43"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8296,11 +8609,11 @@
       <c r="A19" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B19" s="38" t="s">
+      <c r="B19" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="C19" s="39"/>
-      <c r="D19" s="40"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="43"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
#328 Videos(Video list + Video Player) - Team Page
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1410" uniqueCount="427">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="431">
   <si>
     <t>User Profile</t>
   </si>
@@ -1308,13 +1308,6 @@
 101/1/1/1</t>
   </si>
   <si>
-    <t>api/team/teamrosters?team_id=101&amp;sport_id=1
-&amp;complevel_id=1&amp;season_id=1</t>
-  </si>
-  <si>
-    <t>test/team/teamrosters/101/1/1/1</t>
-  </si>
-  <si>
     <t>sportorg/collections/rosters</t>
   </si>
   <si>
@@ -1338,6 +1331,27 @@
   </si>
   <si>
     <t>team/collections/rosters</t>
+  </si>
+  <si>
+    <t>team/collections/videos</t>
+  </si>
+  <si>
+    <t>List of videos associated with team, sport, complevel 
+and season</t>
+  </si>
+  <si>
+    <t>api/team/rosters?team_id=101&amp;sport_id=1
+&amp;complevel_id=1&amp;season_id=1</t>
+  </si>
+  <si>
+    <t>test/team/rosters/101/1/1/1</t>
+  </si>
+  <si>
+    <t>api/team/videos?team_id=101&amp;sport_id =1
+&amp;complevel_id=1&amp;season_id=1</t>
+  </si>
+  <si>
+    <t>test/team/videos/101/1/1/1</t>
   </si>
 </sst>
 </file>
@@ -2139,10 +2153,10 @@
         <v>316</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -4626,7 +4640,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="41" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C2" s="42"/>
       <c r="D2" s="43"/>
@@ -4715,7 +4729,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4750,7 +4764,7 @@
         <v>52</v>
       </c>
       <c r="B23" s="41" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C23" s="42"/>
       <c r="D23" s="43"/>
@@ -4786,7 +4800,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -5084,13 +5098,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L33"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C32" sqref="C32"/>
+      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5826,21 +5840,44 @@
         <v>316</v>
       </c>
       <c r="D33" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="E33" s="17" t="s">
+        <v>417</v>
+      </c>
+      <c r="F33" s="13" t="s">
+        <v>423</v>
+      </c>
+      <c r="G33" s="13" t="s">
+        <v>427</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>428</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="34" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B34" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>425</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="F34" s="13" t="s">
         <v>426</v>
       </c>
-      <c r="E33" s="17" t="s">
-        <v>419</v>
-      </c>
-      <c r="F33" s="13" t="s">
-        <v>425</v>
-      </c>
-      <c r="G33" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>418</v>
-      </c>
-      <c r="J33" s="3" t="s">
+      <c r="G34" s="13" t="s">
+        <v>429</v>
+      </c>
+      <c r="H34" s="9" t="s">
+        <v>430</v>
+      </c>
+      <c r="J34" s="3" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#329, #330 - Images, Fanboard - Team Page
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="431">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="438">
   <si>
     <t>User Profile</t>
   </si>
@@ -1352,6 +1352,30 @@
   </si>
   <si>
     <t>test/team/videos/101/1/1/1</t>
+  </si>
+  <si>
+    <t>team/collections/images</t>
+  </si>
+  <si>
+    <t>team/collections/comments</t>
+  </si>
+  <si>
+    <t>List of images associated with team, sport, complevel 
+and season</t>
+  </si>
+  <si>
+    <t>List of comments associated with team, sport, complevel 
+and season</t>
+  </si>
+  <si>
+    <t>test/team/images/101/1/1/1</t>
+  </si>
+  <si>
+    <t>test/team/comments/101/1/1/1</t>
+  </si>
+  <si>
+    <t>api/team/comments?team_id=101&amp;sport_id =1
+&amp;complevel_id=1&amp;season_id=1</t>
   </si>
 </sst>
 </file>
@@ -5098,13 +5122,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L34"/>
+  <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J34" sqref="J34"/>
+      <selection pane="bottomRight" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5865,7 +5889,7 @@
       <c r="D34" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="E34" s="9" t="s">
+      <c r="E34" s="12" t="s">
         <v>150</v>
       </c>
       <c r="F34" s="13" t="s">
@@ -5878,6 +5902,52 @@
         <v>430</v>
       </c>
       <c r="J34" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>149</v>
+      </c>
+      <c r="F35" s="13" t="s">
+        <v>433</v>
+      </c>
+      <c r="G35" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="H35" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>432</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>434</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>437</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>436</v>
+      </c>
+      <c r="J36" s="3" t="s">
         <v>65</v>
       </c>
     </row>
@@ -5917,6 +5987,9 @@
     <hyperlink ref="E31" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
     <hyperlink ref="E32" location="Sportorg_Teams!A1" display="sportorg/collections/teams"/>
     <hyperlink ref="E33" location="Sportorg_Rosters!A1" display="sportorg/collections/rosters"/>
+    <hyperlink ref="E34" location="Media_Videos!A1" display="media/collections/videos"/>
+    <hyperlink ref="E35" location="Media_Images!A1" display="media/collections/images"/>
+    <hyperlink ref="E36" location="Site_Comments!A1" display="media/collections/comments"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Reg Step1, Game Page(Video, Image List)
I didn't finished still #392.
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -10,34 +10,34 @@
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
     <sheet name="Pages" sheetId="1" r:id="rId2"/>
     <sheet name="User_Basics" sheetId="2" r:id="rId3"/>
-    <sheet name="User_Relateds" sheetId="6" r:id="rId4"/>
-    <sheet name="User_FitnessBasics" sheetId="7" r:id="rId5"/>
-    <sheet name="Site_Comments" sheetId="11" r:id="rId6"/>
-    <sheet name="Site_Pogs" sheetId="15" r:id="rId7"/>
-    <sheet name="Site_Tags" sheetId="16" r:id="rId8"/>
-    <sheet name="Site_Views" sheetId="17" r:id="rId9"/>
-    <sheet name="Site_Votes" sheetId="18" r:id="rId10"/>
-    <sheet name="Sportorg_Sports" sheetId="20" r:id="rId11"/>
-    <sheet name="Sportorg_Positions" sheetId="21" r:id="rId12"/>
-    <sheet name="Sportorg_Complevels" sheetId="22" r:id="rId13"/>
-    <sheet name="Sportorg_Orgs" sheetId="23" r:id="rId14"/>
-    <sheet name="Sportorg_Teams" sheetId="24" r:id="rId15"/>
-    <sheet name="Sportorg_Games" sheetId="25" r:id="rId16"/>
-    <sheet name="Sportorg_Matches" sheetId="26" r:id="rId17"/>
-    <sheet name="Sportorg_Rosters" sheetId="29" r:id="rId18"/>
-    <sheet name="Sportorg_TeamRosters" sheetId="28" r:id="rId19"/>
-    <sheet name="Sportorg_Seasons" sheetId="27" r:id="rId20"/>
-    <sheet name="Media_Videos" sheetId="8" r:id="rId21"/>
-    <sheet name="Media_Images" sheetId="9" r:id="rId22"/>
-    <sheet name="Media_VideoService" sheetId="19" r:id="rId23"/>
+    <sheet name="User_FBReg" sheetId="30" r:id="rId4"/>
+    <sheet name="User_Relateds" sheetId="6" r:id="rId5"/>
+    <sheet name="User_FitnessBasics" sheetId="7" r:id="rId6"/>
+    <sheet name="Site_Comments" sheetId="11" r:id="rId7"/>
+    <sheet name="Site_Pogs" sheetId="15" r:id="rId8"/>
+    <sheet name="Site_Tags" sheetId="16" r:id="rId9"/>
+    <sheet name="Site_Views" sheetId="17" r:id="rId10"/>
+    <sheet name="Site_Votes" sheetId="18" r:id="rId11"/>
+    <sheet name="Sportorg_Sports" sheetId="20" r:id="rId12"/>
+    <sheet name="Sportorg_Positions" sheetId="21" r:id="rId13"/>
+    <sheet name="Sportorg_Complevels" sheetId="22" r:id="rId14"/>
+    <sheet name="Sportorg_Orgs" sheetId="23" r:id="rId15"/>
+    <sheet name="Sportorg_Teams" sheetId="24" r:id="rId16"/>
+    <sheet name="Sportorg_Games" sheetId="25" r:id="rId17"/>
+    <sheet name="Sportorg_Matches" sheetId="26" r:id="rId18"/>
+    <sheet name="Sportorg_Rosters" sheetId="29" r:id="rId19"/>
+    <sheet name="Sportorg_TeamRosters" sheetId="28" r:id="rId20"/>
+    <sheet name="Sportorg_Seasons" sheetId="27" r:id="rId21"/>
+    <sheet name="Media_Videos" sheetId="8" r:id="rId22"/>
+    <sheet name="Media_Images" sheetId="9" r:id="rId23"/>
+    <sheet name="Media_VideoService" sheetId="19" r:id="rId24"/>
   </sheets>
   <calcPr calcId="144525"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1431" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="461">
   <si>
     <t>User Profile</t>
   </si>
@@ -1045,9 +1045,6 @@
     <t>game/collections/comments</t>
   </si>
   <si>
-    <t>List fo video thumbs associated with the game</t>
-  </si>
-  <si>
     <t>List of team rosters associated with the game</t>
   </si>
   <si>
@@ -1380,6 +1377,75 @@
   </si>
   <si>
     <t>test/user/commentsof/101/2</t>
+  </si>
+  <si>
+    <t>Registration</t>
+  </si>
+  <si>
+    <t>register_facebook</t>
+  </si>
+  <si>
+    <t>registration/models/register_facebook</t>
+  </si>
+  <si>
+    <t>user/models/fbreg</t>
+  </si>
+  <si>
+    <t>Facebook registration information</t>
+  </si>
+  <si>
+    <t>api/user/fbreg</t>
+  </si>
+  <si>
+    <t>test/user/fbreg</t>
+  </si>
+  <si>
+    <t>fbreg</t>
+  </si>
+  <si>
+    <t>Facebook Registration Information</t>
+  </si>
+  <si>
+    <t>birth_day</t>
+  </si>
+  <si>
+    <t>high_school</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>removed</t>
+  </si>
+  <si>
+    <t>game/collections/videos</t>
+  </si>
+  <si>
+    <t>List of videos associated with the game</t>
+  </si>
+  <si>
+    <t>List of video thumbs associated with the game</t>
+  </si>
+  <si>
+    <t>api/game/videos?game_id=101</t>
+  </si>
+  <si>
+    <t>test/game/videos/101</t>
+  </si>
+  <si>
+    <t>fb_images</t>
+  </si>
+  <si>
+    <t>registration/collections/fb_images</t>
+  </si>
+  <si>
+    <t>Facebook images</t>
+  </si>
+  <si>
+    <t>api/user/fbimages</t>
+  </si>
+  <si>
+    <t>test/user/fbimages</t>
   </si>
 </sst>
 </file>
@@ -1453,7 +1519,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1473,6 +1539,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -1554,7 +1626,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1622,6 +1694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1638,6 +1711,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -1944,13 +2035,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I31"/>
+  <dimension ref="A1:I32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C1" sqref="C1"/>
+      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1968,10 +2059,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="16" t="s">
         <v>113</v>
       </c>
@@ -2072,220 +2163,228 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B9" s="17"/>
+      <c r="B9" s="17" t="s">
+        <v>445</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>441</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B11" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C11" s="9" t="s">
         <v>200</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D11" s="9" t="s">
         <v>201</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="17" t="s">
-        <v>208</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>209</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="17" t="s">
-        <v>271</v>
+        <v>208</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>272</v>
+        <v>210</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="17" t="s">
-        <v>46</v>
+        <v>271</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>224</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="17" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="17" t="s">
-        <v>83</v>
+        <v>40</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="17" t="s">
-        <v>249</v>
+        <v>83</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B17" s="17" t="s">
-        <v>261</v>
+        <v>249</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>263</v>
+        <v>251</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B18" s="17" t="s">
-        <v>287</v>
+        <v>261</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>300</v>
+        <v>262</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>289</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B19" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>300</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="17" t="s">
         <v>296</v>
       </c>
-      <c r="C19" s="9" t="s">
-        <v>398</v>
-      </c>
-      <c r="D19" s="9" t="s">
+      <c r="C20" s="9" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
+      <c r="D20" s="9" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="17"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="9" t="s">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="B23" s="17" t="s">
         <v>144</v>
       </c>
-      <c r="C22" s="9" t="s">
+      <c r="C23" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D23" s="9" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="17" t="s">
-        <v>154</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="E23" s="13"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="17" t="s">
-        <v>87</v>
+        <v>154</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="E24" s="13"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="17" t="s">
-        <v>170</v>
+        <v>87</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>172</v>
-      </c>
+        <v>166</v>
+      </c>
+      <c r="E25" s="13"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="17" t="s">
+        <v>170</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B27" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C27" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="D26" s="9" t="s">
+      <c r="D27" s="9" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B27" s="17"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="9" t="s">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B28" s="17"/>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B30" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="C29" s="9" t="s">
+      <c r="C30" s="9" t="s">
         <v>138</v>
       </c>
-      <c r="D29" s="9" t="s">
+      <c r="D30" s="9" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B30" s="17" t="s">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C30" s="9" t="s">
+      <c r="C31" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="D30" s="9" t="s">
+      <c r="D31" s="9" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B31" s="12" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C32" s="9" t="s">
         <v>141</v>
       </c>
     </row>
@@ -2302,23 +2401,24 @@
     <hyperlink ref="B6" location="User_Orgs!A1" display="orgs"/>
     <hyperlink ref="B7" location="User_Relateds!A1" display="relateds"/>
     <hyperlink ref="B8" location="User_FitnessBasics!A1" display="fitnessbasics"/>
-    <hyperlink ref="B22" location="Site_Comments!A1" display="comments"/>
-    <hyperlink ref="B29" location="Media_Videos!A1" display="videos"/>
-    <hyperlink ref="B30" location="Media_Images!A1" display="images"/>
-    <hyperlink ref="B23" location="Site_Pogs!A1" display="pogs"/>
-    <hyperlink ref="B24" location="Site_Tags!A1" display="tags"/>
-    <hyperlink ref="B10" location="Sportorg_Sports!A1" display="sports"/>
+    <hyperlink ref="B23" location="Site_Comments!A1" display="comments"/>
+    <hyperlink ref="B30" location="Media_Videos!A1" display="videos"/>
+    <hyperlink ref="B31" location="Media_Images!A1" display="images"/>
+    <hyperlink ref="B24" location="Site_Pogs!A1" display="pogs"/>
+    <hyperlink ref="B25" location="Site_Tags!A1" display="tags"/>
+    <hyperlink ref="B11" location="Sportorg_Sports!A1" display="sports"/>
     <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
-    <hyperlink ref="B11" location="Sportorg_Positions!A1" display="positions"/>
-    <hyperlink ref="B14" location="Sportorg_Teams!A1" display="teams"/>
-    <hyperlink ref="B15" location="Sportorg_Games!A1" display="games"/>
-    <hyperlink ref="B16" location="Sportorg_Matches!A1" display="matches"/>
-    <hyperlink ref="B17" location="Sportorg_Seasons!A1" display="seasons"/>
-    <hyperlink ref="B13" location="Sportorg_Orgs!A1" display="orgs"/>
-    <hyperlink ref="B12" location="Sportorg_Complevels!A1" display="complevels"/>
-    <hyperlink ref="B18" location="Sportorg_TeamRosters!A1" display="teamrosters"/>
-    <hyperlink ref="B31" location="Media_VideoService!A1" display="videoservice"/>
-    <hyperlink ref="B19" location="Sportorg_Rosters!A1" display="rosters"/>
+    <hyperlink ref="B12" location="Sportorg_Positions!A1" display="positions"/>
+    <hyperlink ref="B15" location="Sportorg_Teams!A1" display="teams"/>
+    <hyperlink ref="B16" location="Sportorg_Games!A1" display="games"/>
+    <hyperlink ref="B17" location="Sportorg_Matches!A1" display="matches"/>
+    <hyperlink ref="B18" location="Sportorg_Seasons!A1" display="seasons"/>
+    <hyperlink ref="B14" location="Sportorg_Orgs!A1" display="orgs"/>
+    <hyperlink ref="B13" location="Sportorg_Complevels!A1" display="complevels"/>
+    <hyperlink ref="B19" location="Sportorg_TeamRosters!A1" display="teamrosters"/>
+    <hyperlink ref="B32" location="Media_VideoService!A1" display="videoservice"/>
+    <hyperlink ref="B20" location="Sportorg_Rosters!A1" display="rosters"/>
+    <hyperlink ref="B9" location="User_FBReg!A1" display="fbreg"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2344,14 +2444,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2360,11 +2460,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>197</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="42" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2418,7 +2518,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>14</v>
@@ -2429,7 +2529,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="15" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>14</v>
@@ -2449,7 +2549,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2483,11 +2583,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2520,7 +2620,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -2566,6 +2666,247 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:B29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
+    <col min="2" max="2" width="15" style="15" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="15"/>
+    <col min="5" max="5" width="13.85546875" style="15" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="15" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="14">
+        <v>41351</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>197</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="15" t="s">
+        <v>147</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="15" t="s">
+        <v>148</v>
+      </c>
+      <c r="E5" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="15" t="s">
+        <v>161</v>
+      </c>
+      <c r="E7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F16" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
+      <c r="E19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="E22" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="E25" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F25" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="F26" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B19:D19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -2586,14 +2927,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2602,11 +2943,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2682,12 +3023,12 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="15" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E10" s="15" t="s">
         <v>14</v>
@@ -2695,7 +3036,7 @@
     </row>
     <row r="11" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C11" s="29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E11" s="29" t="s">
         <v>14</v>
@@ -2704,7 +3045,7 @@
     </row>
     <row r="12" spans="1:7" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C12" s="29" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E12" s="29" t="s">
         <v>14</v>
@@ -2756,11 +3097,11 @@
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="42" t="s">
         <v>203</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -2825,7 +3166,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -2833,7 +3174,7 @@
         <v>41367</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -2851,7 +3192,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -2872,14 +3213,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2888,11 +3229,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3022,11 +3363,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3104,7 +3445,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -3125,14 +3466,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -3141,11 +3482,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3253,11 +3594,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>269</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3341,7 +3682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G28"/>
   <sheetViews>
@@ -3362,14 +3703,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3378,11 +3719,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3532,11 +3873,11 @@
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="41" t="s">
+      <c r="B21" s="42" t="s">
         <v>226</v>
       </c>
-      <c r="C21" s="42"/>
-      <c r="D21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="44"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3614,7 +3955,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G49"/>
   <sheetViews>
@@ -3635,14 +3976,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3651,11 +3992,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3722,7 +4063,7 @@
     </row>
     <row r="9" spans="1:7" s="31" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C9" s="31" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>21</v>
@@ -3749,7 +4090,7 @@
     </row>
     <row r="12" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C12" s="34" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>21</v>
@@ -3758,7 +4099,7 @@
     </row>
     <row r="13" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C13" s="34" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E13" s="34" t="s">
         <v>14</v>
@@ -3776,7 +4117,7 @@
     </row>
     <row r="15" spans="1:7" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C15" s="34" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>21</v>
@@ -3922,11 +4263,11 @@
       <c r="A35" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="41" t="s">
+      <c r="B35" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="C35" s="42"/>
-      <c r="D35" s="43"/>
+      <c r="C35" s="43"/>
+      <c r="D35" s="44"/>
       <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
@@ -3999,23 +4340,23 @@
         <v>41362</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B46" s="20" t="s">
+        <v>350</v>
+      </c>
+      <c r="E46" s="20" t="s">
         <v>351</v>
-      </c>
-      <c r="E46" s="20" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B47" s="20" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E47" s="20" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -4023,7 +4364,7 @@
         <v>41367</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -4031,7 +4372,7 @@
         <v>41369</v>
       </c>
       <c r="B49" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>
@@ -4049,7 +4390,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G36"/>
   <sheetViews>
@@ -4070,14 +4411,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -4086,11 +4427,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4188,7 +4529,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="20" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E13" s="20" t="s">
         <v>21</v>
@@ -4196,13 +4537,13 @@
     </row>
     <row r="14" spans="1:7" s="30" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C14" s="30" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>14</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -4258,11 +4599,11 @@
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="42" t="s">
         <v>236</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4368,7 +4709,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -4389,14 +4730,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4405,11 +4746,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4548,11 +4889,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4630,7 +4971,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -4651,14 +4992,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4667,11 +5008,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>399</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="42" t="s">
+        <v>398</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4757,7 +5098,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -4791,11 +5132,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="41" t="s">
-        <v>400</v>
-      </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
+      <c r="B23" s="42" t="s">
+        <v>399</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4828,7 +5169,7 @@
         <v>14</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -4852,257 +5193,6 @@
         <v>28</v>
       </c>
       <c r="E30" s="36" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B23:D23"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
-    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G30"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" style="23" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="23" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" style="23" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" style="23" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" style="23" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="23"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="14">
-        <v>41352</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>294</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
-        <v>295</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="23" t="s">
-        <v>280</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
-        <v>296</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" s="23" t="s">
-        <v>55</v>
-      </c>
-      <c r="E7" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C8" s="23" t="s">
-        <v>297</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="23" t="s">
-        <v>109</v>
-      </c>
-      <c r="E9" s="22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="23" t="s">
-        <v>298</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E16" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F19" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E20" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="F20" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B23" s="41" t="s">
-        <v>299</v>
-      </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
-      <c r="E23" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="23" t="s">
-        <v>10</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" s="23" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="23" t="s">
-        <v>14</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="23" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="23" t="s">
-        <v>27</v>
-      </c>
-      <c r="F29" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="E30" s="23" t="s">
         <v>29</v>
       </c>
       <c r="F30" s="6" t="b">
@@ -5126,20 +5216,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L36"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="E3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G12" sqref="G12"/>
+      <selection pane="bottomRight" activeCell="J40" sqref="J40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.5703125" style="9" customWidth="1"/>
     <col min="2" max="2" width="19.85546875" style="9" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="36.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" style="9" customWidth="1"/>
     <col min="6" max="7" width="53.7109375" style="9" bestFit="1" customWidth="1"/>
@@ -5152,10 +5242,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="39"/>
+      <c r="B1" s="40"/>
       <c r="C1" s="16" t="s">
         <v>113</v>
       </c>
@@ -5281,13 +5371,13 @@
         <v>224</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>59</v>
@@ -5304,13 +5394,13 @@
         <v>58</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="G7" s="9" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>59</v>
@@ -5327,13 +5417,13 @@
         <v>74</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="J8" s="3" t="s">
         <v>59</v>
@@ -5350,13 +5440,13 @@
         <v>130</v>
       </c>
       <c r="F9" s="9" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J9" s="3" t="s">
         <v>59</v>
@@ -5373,13 +5463,13 @@
         <v>129</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="H10" s="9" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="J10" s="3" t="s">
         <v>59</v>
@@ -5396,13 +5486,13 @@
         <v>138</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="J11" s="3" t="s">
         <v>59</v>
@@ -5419,13 +5509,13 @@
         <v>142</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="J12" s="3" t="s">
         <v>59</v>
@@ -5506,7 +5596,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="9" t="s">
         <v>287</v>
       </c>
@@ -5517,7 +5607,7 @@
         <v>289</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G17" s="9" t="s">
         <v>290</v>
@@ -5529,119 +5619,131 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="9" t="s">
+    <row r="18" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="46" t="s">
+        <v>450</v>
+      </c>
+      <c r="B18" s="46" t="s">
         <v>301</v>
       </c>
-      <c r="C18" s="9" t="s">
+      <c r="C18" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="E18" s="12" t="s">
+      <c r="E18" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="G18" s="9" t="s">
+      <c r="G18" s="46" t="s">
         <v>304</v>
       </c>
-      <c r="H18" s="9" t="s">
+      <c r="H18" s="46" t="s">
         <v>305</v>
       </c>
-      <c r="J18" s="3" t="s">
+      <c r="I18" s="48"/>
+      <c r="J18" s="48" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="9" t="s">
+      <c r="K18" s="48"/>
+      <c r="L18" s="48"/>
+    </row>
+    <row r="19" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="46" t="s">
+        <v>450</v>
+      </c>
+      <c r="B19" s="46" t="s">
         <v>313</v>
       </c>
-      <c r="D19" s="9" t="s">
+      <c r="D19" s="46" t="s">
         <v>314</v>
       </c>
-      <c r="E19" s="12" t="s">
+      <c r="E19" s="47" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="9" t="s">
-        <v>332</v>
-      </c>
-      <c r="G19" s="9" t="s">
+      <c r="F19" s="46" t="s">
+        <v>453</v>
+      </c>
+      <c r="G19" s="46" t="s">
         <v>315</v>
       </c>
-      <c r="H19" s="9" t="s">
+      <c r="H19" s="46" t="s">
         <v>316</v>
       </c>
-      <c r="J19" s="3" t="s">
+      <c r="I19" s="48"/>
+      <c r="J19" s="48" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="9" t="s">
+      <c r="K19" s="48"/>
+      <c r="L19" s="48"/>
+    </row>
+    <row r="20" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="49" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="49" t="s">
+        <v>451</v>
+      </c>
+      <c r="E20" s="50" t="s">
+        <v>130</v>
+      </c>
+      <c r="F20" s="49" t="s">
+        <v>452</v>
+      </c>
+      <c r="G20" s="49" t="s">
+        <v>454</v>
+      </c>
+      <c r="H20" s="49" t="s">
+        <v>455</v>
+      </c>
+      <c r="I20" s="51"/>
+      <c r="J20" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="K20" s="51"/>
+      <c r="L20" s="51"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B21" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="D20" s="9" t="s">
+      <c r="D21" s="9" t="s">
         <v>317</v>
       </c>
-      <c r="E20" s="12" t="s">
+      <c r="E21" s="12" t="s">
         <v>129</v>
       </c>
-      <c r="F20" s="9" t="s">
+      <c r="F21" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="G20" s="9" t="s">
+      <c r="G21" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="H20" s="9" t="s">
+      <c r="H21" s="9" t="s">
         <v>320</v>
-      </c>
-      <c r="J20" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="9" t="s">
-        <v>321</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="E21" s="12" t="s">
-        <v>138</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>324</v>
-      </c>
-      <c r="H21" s="9" t="s">
-        <v>325</v>
       </c>
       <c r="J21" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F22" s="9" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="G22" s="9" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="H22" s="9" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="J22" s="3" t="s">
         <v>59</v>
@@ -5650,308 +5752,383 @@
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>331</v>
+        <v>326</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>327</v>
       </c>
       <c r="E23" s="12" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="G23" s="9" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="H23" s="9" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="J23" s="3" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K23" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B24" s="9" t="s">
-        <v>337</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>338</v>
+        <v>144</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>331</v>
       </c>
       <c r="E24" s="12" t="s">
         <v>142</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="G24" s="9" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="H24" s="9" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="J24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="K24" s="3" t="s">
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B25" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C25" s="9" t="s">
+        <v>337</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>142</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>339</v>
+      </c>
+      <c r="H25" s="9" t="s">
+        <v>340</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K25" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="9" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="9" t="s">
+        <v>345</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>346</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="E27" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="F27" s="9" t="s">
         <v>347</v>
       </c>
-      <c r="E26" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="F26" s="9" t="s">
+      <c r="G27" s="9" t="s">
         <v>348</v>
       </c>
-      <c r="G26" s="9" t="s">
+      <c r="H27" s="9" t="s">
         <v>349</v>
-      </c>
-      <c r="H26" s="9" t="s">
-        <v>350</v>
-      </c>
-      <c r="J26" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B27" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="E27" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>360</v>
-      </c>
-      <c r="G27" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="H27" s="9" t="s">
-        <v>362</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="9" t="s">
-        <v>271</v>
+        <v>20</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
       <c r="E28" s="12" t="s">
-        <v>272</v>
+        <v>201</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
       <c r="G28" s="9" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="H28" s="9" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="J28" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="9" t="s">
-        <v>261</v>
+        <v>271</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>374</v>
+        <v>362</v>
       </c>
       <c r="E29" s="12" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>375</v>
+        <v>363</v>
       </c>
       <c r="G29" s="9" t="s">
-        <v>383</v>
+        <v>364</v>
       </c>
       <c r="H29" s="9" t="s">
-        <v>376</v>
+        <v>365</v>
       </c>
       <c r="J29" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>379</v>
+        <v>261</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="E30" s="12" t="s">
-        <v>242</v>
-      </c>
-      <c r="F30" s="13" t="s">
-        <v>384</v>
-      </c>
-      <c r="G30" s="13" t="s">
-        <v>386</v>
-      </c>
-      <c r="H30" s="13" t="s">
-        <v>387</v>
+        <v>263</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>374</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>382</v>
+      </c>
+      <c r="H30" s="9" t="s">
+        <v>375</v>
       </c>
       <c r="J30" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>242</v>
       </c>
       <c r="F31" s="13" t="s">
+        <v>383</v>
+      </c>
+      <c r="G31" s="13" t="s">
         <v>385</v>
       </c>
-      <c r="G31" s="13" t="s">
-        <v>388</v>
-      </c>
       <c r="H31" s="13" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="B32" s="9" t="s">
-        <v>392</v>
+        <v>380</v>
       </c>
       <c r="D32" s="9" t="s">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="E32" s="12" t="s">
-        <v>234</v>
+        <v>242</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>394</v>
+        <v>384</v>
       </c>
       <c r="G32" s="13" t="s">
-        <v>395</v>
+        <v>387</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>396</v>
+        <v>388</v>
       </c>
       <c r="J32" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
-        <v>296</v>
+        <v>391</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>404</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>397</v>
+        <v>392</v>
+      </c>
+      <c r="E33" s="12" t="s">
+        <v>234</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>403</v>
+        <v>393</v>
       </c>
       <c r="G33" s="13" t="s">
-        <v>407</v>
-      </c>
-      <c r="H33" s="9" t="s">
-        <v>408</v>
+        <v>394</v>
+      </c>
+      <c r="H33" s="13" t="s">
+        <v>395</v>
       </c>
       <c r="J33" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>78</v>
+        <v>296</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>405</v>
-      </c>
-      <c r="E34" s="12" t="s">
-        <v>130</v>
+        <v>403</v>
+      </c>
+      <c r="E34" s="17" t="s">
+        <v>396</v>
       </c>
       <c r="F34" s="13" t="s">
+        <v>402</v>
+      </c>
+      <c r="G34" s="13" t="s">
         <v>406</v>
       </c>
-      <c r="G34" s="13" t="s">
-        <v>409</v>
-      </c>
       <c r="H34" s="9" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="J34" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="E35" s="12" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>413</v>
+        <v>405</v>
       </c>
       <c r="G35" s="13" t="s">
-        <v>417</v>
+        <v>408</v>
       </c>
       <c r="H35" s="9" t="s">
-        <v>415</v>
+        <v>409</v>
       </c>
       <c r="J35" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>410</v>
+      </c>
+      <c r="E36" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F36" s="13" t="s">
+        <v>412</v>
+      </c>
+      <c r="G36" s="13" t="s">
+        <v>416</v>
+      </c>
+      <c r="H36" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B37" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="D36" s="9" t="s">
-        <v>412</v>
-      </c>
-      <c r="E36" s="12" t="s">
+      <c r="D37" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="E37" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="F36" s="13" t="s">
-        <v>414</v>
-      </c>
-      <c r="G36" s="13" t="s">
-        <v>417</v>
-      </c>
-      <c r="H36" s="9" t="s">
+      <c r="F37" s="13" t="s">
+        <v>413</v>
+      </c>
+      <c r="G37" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="J36" s="3" t="s">
+      <c r="H37" s="9" t="s">
+        <v>415</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" s="9" t="s">
+        <v>438</v>
+      </c>
+      <c r="B39" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="C39" s="9" t="s">
+        <v>440</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>442</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>443</v>
+      </c>
+      <c r="H39" s="9" t="s">
+        <v>444</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B40" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="D40" s="9" t="s">
+        <v>457</v>
+      </c>
+      <c r="E40" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>459</v>
+      </c>
+      <c r="H40" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="J40" s="3" t="s">
         <v>59</v>
       </c>
     </row>
@@ -5978,28 +6155,281 @@
     <hyperlink ref="E7" location="User_Relateds!A1" display="user/collections/relateds"/>
     <hyperlink ref="E8" location="User_FitnessBasics!A1" display="user/collections/fitnessbasics"/>
     <hyperlink ref="E19" location="Media_Videos!A1" display="media/collections/videos"/>
-    <hyperlink ref="E20" location="Media_Images!A1" display="media/collections/images"/>
-    <hyperlink ref="E21" location="Media_Videos!A1" display="media/models/video"/>
-    <hyperlink ref="E22" location="Media_Images!A1" display="media/models/image"/>
-    <hyperlink ref="E23" location="Site_Comments!A1" display="site/collections/comments"/>
+    <hyperlink ref="E21" location="Media_Images!A1" display="media/collections/images"/>
+    <hyperlink ref="E22" location="Media_Videos!A1" display="media/models/video"/>
+    <hyperlink ref="E23" location="Media_Images!A1" display="media/models/image"/>
     <hyperlink ref="E24" location="Site_Comments!A1" display="site/collections/comments"/>
-    <hyperlink ref="E26" location="Sportorg_Teams!A1" display="sportorg/models/team"/>
-    <hyperlink ref="E27" location="Sportorg_Sports!A1" display="sportorg/collections/sports"/>
-    <hyperlink ref="E28" location="Sportorg_Complevels!A1" display="sportorg/collections/complevels"/>
-    <hyperlink ref="E29" location="Sportorg_Seasons!A1" display="sportorg/collections/seasons"/>
-    <hyperlink ref="E30" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
+    <hyperlink ref="E25" location="Site_Comments!A1" display="site/collections/comments"/>
+    <hyperlink ref="E27" location="Sportorg_Teams!A1" display="sportorg/models/team"/>
+    <hyperlink ref="E28" location="Sportorg_Sports!A1" display="sportorg/collections/sports"/>
+    <hyperlink ref="E29" location="Sportorg_Complevels!A1" display="sportorg/collections/complevels"/>
+    <hyperlink ref="E30" location="Sportorg_Seasons!A1" display="sportorg/collections/seasons"/>
     <hyperlink ref="E31" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
-    <hyperlink ref="E32" location="Sportorg_Teams!A1" display="sportorg/collections/teams"/>
-    <hyperlink ref="E33" location="Sportorg_Rosters!A1" display="sportorg/collections/rosters"/>
-    <hyperlink ref="E34" location="Media_Videos!A1" display="media/collections/videos"/>
-    <hyperlink ref="E35" location="Media_Images!A1" display="media/collections/images"/>
-    <hyperlink ref="E36" location="Site_Comments!A1" display="media/collections/comments"/>
+    <hyperlink ref="E32" location="Sportorg_Games!A1" display="sportorg/collections/games"/>
+    <hyperlink ref="E33" location="Sportorg_Teams!A1" display="sportorg/collections/teams"/>
+    <hyperlink ref="E34" location="Sportorg_Rosters!A1" display="sportorg/collections/rosters"/>
+    <hyperlink ref="E35" location="Media_Videos!A1" display="media/collections/videos"/>
+    <hyperlink ref="E36" location="Media_Images!A1" display="media/collections/images"/>
+    <hyperlink ref="E37" location="Site_Comments!A1" display="media/collections/comments"/>
+    <hyperlink ref="E39" location="User_FBReg!A1" display="user/models/fbreg"/>
+    <hyperlink ref="E20" location="Media_Videos!A1" display="media/collections/videos"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G30"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="23" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="23" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" style="23" customWidth="1"/>
+    <col min="4" max="4" width="12.7109375" style="23" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" style="23" customWidth="1"/>
+    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="23" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="14">
+        <v>41352</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>294</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
+        <v>295</v>
+      </c>
+      <c r="E4" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="23" t="s">
+        <v>280</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="23" t="s">
+        <v>296</v>
+      </c>
+      <c r="E6" s="23" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C7" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="23" t="s">
+        <v>297</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="23" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" s="23" t="s">
+        <v>298</v>
+      </c>
+      <c r="E10" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B19" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E19" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F19" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E20" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="42" t="s">
+        <v>299</v>
+      </c>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="23" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="23" t="s">
+        <v>11</v>
+      </c>
+      <c r="E26" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="F26" s="7" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" s="23" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>27</v>
+      </c>
+      <c r="F29" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B23:D23"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
@@ -6020,14 +6450,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -6036,11 +6466,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6061,7 +6491,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="20" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E4" s="20" t="s">
         <v>21</v>
@@ -6129,11 +6559,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="41" t="s">
+      <c r="B23" s="42" t="s">
         <v>265</v>
       </c>
-      <c r="C23" s="42"/>
-      <c r="D23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="44"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -6211,7 +6641,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G48"/>
   <sheetViews>
@@ -6230,24 +6660,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6550,11 +6980,11 @@
       <c r="A37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="41" t="s">
+      <c r="B37" s="42" t="s">
         <v>133</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="43"/>
+      <c r="C37" s="43"/>
+      <c r="D37" s="44"/>
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
@@ -6646,7 +7076,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G25"/>
   <sheetViews>
@@ -6664,24 +7094,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6790,11 +7220,11 @@
       <c r="A17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="41" t="s">
+      <c r="B17" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="44"/>
       <c r="E17" s="2" t="s">
         <v>17</v>
       </c>
@@ -6806,12 +7236,12 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="44"/>
-      <c r="D18" s="44"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
+      <c r="A18" s="45"/>
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="45"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -6880,7 +7310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
@@ -6901,24 +7331,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>342</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="42" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6942,7 +7372,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="27" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E5" s="27" t="s">
         <v>21</v>
@@ -6958,7 +7388,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="27" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>14</v>
@@ -7010,11 +7440,11 @@
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="41" t="s">
-        <v>343</v>
-      </c>
-      <c r="C16" s="42"/>
-      <c r="D16" s="43"/>
+      <c r="B16" s="42" t="s">
+        <v>342</v>
+      </c>
+      <c r="C16" s="43"/>
+      <c r="D16" s="44"/>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
@@ -7122,14 +7552,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>184</v>
@@ -7139,11 +7569,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7316,6 +7746,174 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" style="39" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="39" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="39"/>
+    <col min="5" max="5" width="13.85546875" style="39" customWidth="1"/>
+    <col min="6" max="6" width="38.5703125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="62.28515625" style="39" customWidth="1"/>
+    <col min="8" max="8" width="12.85546875" style="39" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="39"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="41" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="41"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="6" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>441</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="39" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="39" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6" s="39" t="s">
+        <v>447</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="39" t="s">
+        <v>448</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="39" t="s">
+        <v>449</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="39" t="s">
+        <v>297</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="39" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="39" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="39" t="s">
+        <v>26</v>
+      </c>
+      <c r="E17" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="F17" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="39" t="s">
+        <v>28</v>
+      </c>
+      <c r="E18" s="39" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="14"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="B2:D2"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
+    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G31"/>
   <sheetViews>
@@ -7334,18 +7932,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7530,11 +8128,11 @@
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="42" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="44"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -7607,13 +8205,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7628,18 +8226,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40"/>
-      <c r="B1" s="40"/>
+      <c r="A1" s="41"/>
+      <c r="B1" s="41"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7736,11 +8334,11 @@
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="41" t="s">
+      <c r="B15" s="42" t="s">
         <v>188</v>
       </c>
-      <c r="C15" s="42"/>
-      <c r="D15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="44"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -7810,7 +8408,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
@@ -7829,14 +8427,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -7845,11 +8443,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7993,11 +8591,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -8075,7 +8673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
@@ -8095,14 +8693,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -8111,11 +8709,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="42" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8234,11 +8832,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="41" t="s">
+      <c r="B19" s="42" t="s">
         <v>191</v>
       </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -8317,236 +8915,6 @@
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="18" t="s">
         <v>110</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B19:D19"/>
-  </mergeCells>
-  <hyperlinks>
-    <hyperlink ref="A1:B1" location="Packages!A1" display="Packages"/>
-    <hyperlink ref="C1:D1" location="Pages!A1" display="Pages"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="15" style="15" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" style="15"/>
-    <col min="5" max="5" width="13.85546875" style="15" customWidth="1"/>
-    <col min="6" max="6" width="41.140625" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="62.28515625" style="15" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
-        <v>112</v>
-      </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="40"/>
-      <c r="E1" s="14">
-        <v>41351</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="41" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="15" t="s">
-        <v>147</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="15" t="s">
-        <v>148</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="15" t="s">
-        <v>149</v>
-      </c>
-      <c r="E6" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="15" t="s">
-        <v>161</v>
-      </c>
-      <c r="E7" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E12" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F12" s="7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F15" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E16" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F16" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B19" s="41" t="s">
-        <v>194</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
-      <c r="E19" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="15" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="E22" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F22" s="7" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
-        <v>26</v>
-      </c>
-      <c r="E25" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="E26" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="F26" s="6" t="b">
-        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -8569,7 +8937,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29:B29"/>
+      <selection activeCell="A29" sqref="A29:B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8584,14 +8952,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="41" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40" t="s">
+      <c r="B1" s="41"/>
+      <c r="C1" s="41" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="40"/>
+      <c r="D1" s="41"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -8600,11 +8968,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="41" t="s">
-        <v>195</v>
-      </c>
-      <c r="C2" s="42"/>
-      <c r="D2" s="43"/>
+      <c r="B2" s="42" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="43"/>
+      <c r="D2" s="44"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8658,23 +9026,12 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="15" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="E7" s="15" t="s">
         <v>14</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="15" t="s">
-        <v>175</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="F8" s="6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -8689,7 +9046,7 @@
         <v>14</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -8723,11 +9080,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="41" t="s">
-        <v>196</v>
-      </c>
-      <c r="C19" s="42"/>
-      <c r="D19" s="43"/>
+      <c r="B19" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C19" s="43"/>
+      <c r="D19" s="44"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -8760,7 +9117,7 @@
         <v>14</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
#392 - Use Facebook Image
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="16" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1488" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="471">
   <si>
     <t>User Profile</t>
   </si>
@@ -1446,6 +1446,36 @@
   </si>
   <si>
     <t>test/user/fbimages</t>
+  </si>
+  <si>
+    <t>use_fb_image</t>
+  </si>
+  <si>
+    <t>Submit selected fb image</t>
+  </si>
+  <si>
+    <t>api/user/fbselectimage</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>crop_x</t>
+  </si>
+  <si>
+    <t>crop_y</t>
+  </si>
+  <si>
+    <t>crop_width</t>
+  </si>
+  <si>
+    <t>crop_height</t>
+  </si>
+  <si>
+    <t>image_width</t>
+  </si>
+  <si>
+    <t>image_height</t>
   </si>
 </sst>
 </file>
@@ -1626,7 +1656,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="2"/>
@@ -1695,21 +1725,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1729,6 +1744,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Bad" xfId="5" builtinId="27"/>
@@ -2059,10 +2090,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="16" t="s">
         <v>113</v>
       </c>
@@ -2444,14 +2475,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2460,11 +2491,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>195</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2583,11 +2614,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2685,14 +2716,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2701,11 +2732,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -2824,11 +2855,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>196</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -2927,14 +2958,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -2943,11 +2974,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>202</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3097,11 +3128,11 @@
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="49" t="s">
         <v>203</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3213,14 +3244,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -3229,11 +3260,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>211</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3363,11 +3394,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>214</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3466,14 +3497,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -3482,11 +3513,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>219</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3594,11 +3625,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>269</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -3703,14 +3734,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3719,11 +3750,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>225</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -3873,11 +3904,11 @@
       <c r="A21" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="49" t="s">
         <v>226</v>
       </c>
-      <c r="C21" s="43"/>
-      <c r="D21" s="44"/>
+      <c r="C21" s="50"/>
+      <c r="D21" s="51"/>
       <c r="E21" s="2" t="s">
         <v>17</v>
       </c>
@@ -3976,14 +4007,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -3992,11 +4023,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>235</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4263,11 +4294,11 @@
       <c r="A35" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B35" s="42" t="s">
+      <c r="B35" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="C35" s="43"/>
-      <c r="D35" s="44"/>
+      <c r="C35" s="50"/>
+      <c r="D35" s="51"/>
       <c r="E35" s="2" t="s">
         <v>17</v>
       </c>
@@ -4411,14 +4442,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41353</v>
       </c>
@@ -4427,11 +4458,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4599,11 +4630,11 @@
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="49" t="s">
         <v>236</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -4730,14 +4761,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -4746,11 +4777,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>252</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -4889,11 +4920,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="49" t="s">
         <v>253</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -4992,14 +5023,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -5008,11 +5039,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>398</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -5132,11 +5163,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="49" t="s">
         <v>399</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -5216,13 +5247,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="J40" sqref="J40"/>
+      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5242,10 +5273,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="47" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="40"/>
+      <c r="B1" s="47"/>
       <c r="C1" s="16" t="s">
         <v>113</v>
       </c>
@@ -5619,89 +5650,89 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="46" t="s">
+    <row r="18" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="41" t="s">
         <v>450</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="41" t="s">
         <v>301</v>
       </c>
-      <c r="C18" s="46" t="s">
+      <c r="C18" s="41" t="s">
         <v>302</v>
       </c>
-      <c r="E18" s="47" t="s">
+      <c r="E18" s="42" t="s">
         <v>138</v>
       </c>
-      <c r="F18" s="46" t="s">
+      <c r="F18" s="41" t="s">
         <v>303</v>
       </c>
-      <c r="G18" s="46" t="s">
+      <c r="G18" s="41" t="s">
         <v>304</v>
       </c>
-      <c r="H18" s="46" t="s">
+      <c r="H18" s="41" t="s">
         <v>305</v>
       </c>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48" t="s">
+      <c r="I18" s="43"/>
+      <c r="J18" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="K18" s="48"/>
-      <c r="L18" s="48"/>
-    </row>
-    <row r="19" spans="1:12" s="46" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="46" t="s">
+      <c r="K18" s="43"/>
+      <c r="L18" s="43"/>
+    </row>
+    <row r="19" spans="1:12" s="41" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="41" t="s">
         <v>450</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="41" t="s">
         <v>313</v>
       </c>
-      <c r="D19" s="46" t="s">
+      <c r="D19" s="41" t="s">
         <v>314</v>
       </c>
-      <c r="E19" s="47" t="s">
+      <c r="E19" s="42" t="s">
         <v>130</v>
       </c>
-      <c r="F19" s="46" t="s">
+      <c r="F19" s="41" t="s">
         <v>453</v>
       </c>
-      <c r="G19" s="46" t="s">
+      <c r="G19" s="41" t="s">
         <v>315</v>
       </c>
-      <c r="H19" s="46" t="s">
+      <c r="H19" s="41" t="s">
         <v>316</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48" t="s">
+      <c r="I19" s="43"/>
+      <c r="J19" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="K19" s="48"/>
-      <c r="L19" s="48"/>
-    </row>
-    <row r="20" spans="1:12" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="49" t="s">
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+    </row>
+    <row r="20" spans="1:12" s="44" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="44" t="s">
         <v>451</v>
       </c>
-      <c r="E20" s="50" t="s">
+      <c r="E20" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="44" t="s">
         <v>452</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="44" t="s">
         <v>454</v>
       </c>
-      <c r="H20" s="49" t="s">
+      <c r="H20" s="44" t="s">
         <v>455</v>
       </c>
-      <c r="I20" s="51"/>
-      <c r="J20" s="51" t="s">
+      <c r="I20" s="46"/>
+      <c r="J20" s="46" t="s">
         <v>59</v>
       </c>
-      <c r="K20" s="51"/>
-      <c r="L20" s="51"/>
+      <c r="K20" s="46"/>
+      <c r="L20" s="46"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="9" t="s">
@@ -5968,7 +5999,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="9" t="s">
         <v>391</v>
       </c>
@@ -5991,7 +6022,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
         <v>296</v>
       </c>
@@ -6014,7 +6045,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B35" s="9" t="s">
         <v>78</v>
       </c>
@@ -6037,7 +6068,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="36" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B36" s="9" t="s">
         <v>92</v>
       </c>
@@ -6060,7 +6091,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
         <v>144</v>
       </c>
@@ -6083,7 +6114,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="9" t="s">
         <v>438</v>
       </c>
@@ -6109,14 +6140,14 @@
         <v>59</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
         <v>456</v>
       </c>
       <c r="D40" s="9" t="s">
         <v>457</v>
       </c>
-      <c r="E40" s="9" t="s">
+      <c r="E40" s="12" t="s">
         <v>129</v>
       </c>
       <c r="F40" s="9" t="s">
@@ -6130,6 +6161,26 @@
       </c>
       <c r="J40" s="3" t="s">
         <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B41" s="9" t="s">
+        <v>461</v>
+      </c>
+      <c r="E41" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F41" s="9" t="s">
+        <v>462</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>463</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="K41" s="3" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -6173,6 +6224,8 @@
     <hyperlink ref="E37" location="Site_Comments!A1" display="media/collections/comments"/>
     <hyperlink ref="E39" location="User_FBReg!A1" display="user/models/fbreg"/>
     <hyperlink ref="E20" location="Media_Videos!A1" display="media/collections/videos"/>
+    <hyperlink ref="E41" location="Media_Images!A1" display="media/collections/images"/>
+    <hyperlink ref="E40" location="Media_Images!A1" display="media/collections/images"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -6199,14 +6252,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -6215,11 +6268,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>294</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6347,11 +6400,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="49" t="s">
         <v>299</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -6450,14 +6503,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41352</v>
       </c>
@@ -6466,11 +6519,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>264</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6559,11 +6612,11 @@
       <c r="A23" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="42" t="s">
+      <c r="B23" s="49" t="s">
         <v>265</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="50"/>
+      <c r="D23" s="51"/>
       <c r="E23" s="2" t="s">
         <v>17</v>
       </c>
@@ -6660,24 +6713,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>132</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -6980,11 +7033,11 @@
       <c r="A37" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="49" t="s">
         <v>133</v>
       </c>
-      <c r="C37" s="43"/>
-      <c r="D37" s="44"/>
+      <c r="C37" s="50"/>
+      <c r="D37" s="51"/>
       <c r="E37" s="2" t="s">
         <v>17</v>
       </c>
@@ -7078,10 +7131,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7094,24 +7147,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>198</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7177,119 +7230,191 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F10" s="7"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>25</v>
+    <row r="9" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F9" s="6"/>
+    </row>
+    <row r="10" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>465</v>
+      </c>
+      <c r="E10" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="40" t="s">
+        <v>466</v>
+      </c>
+      <c r="E11" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="40" t="s">
+        <v>467</v>
+      </c>
+      <c r="E12" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F12" s="6">
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E13" t="s">
-        <v>27</v>
+        <v>468</v>
+      </c>
+      <c r="E13" s="40" t="s">
+        <v>21</v>
       </c>
       <c r="F13" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
-      <c r="F14" s="6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B17" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="C17" s="43"/>
-      <c r="D17" s="44"/>
-      <c r="E17" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="45"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
+    <row r="14" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="40" t="s">
+        <v>469</v>
+      </c>
+      <c r="E14" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F14" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="40" t="s">
+        <v>470</v>
+      </c>
+      <c r="E15" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="6"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" t="s">
+        <v>14</v>
+      </c>
+      <c r="F17" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="E20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F20" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" t="s">
+        <v>29</v>
+      </c>
+      <c r="F21" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" s="49" t="s">
+        <v>199</v>
+      </c>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
+      <c r="E24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="52"/>
+      <c r="B25" s="52"/>
+      <c r="C25" s="52"/>
+      <c r="D25" s="52"/>
+      <c r="E25" s="52"/>
+      <c r="F25" s="52"/>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>22</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B28" t="s">
         <v>11</v>
       </c>
-      <c r="E21" t="s">
-        <v>14</v>
-      </c>
-      <c r="F21" s="7"/>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+      <c r="F28" s="7"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
         <v>26</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E31" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="F31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="E25" t="s">
+      <c r="E32" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="6" t="b">
+      <c r="F32" s="6" t="b">
         <v>0</v>
       </c>
     </row>
@@ -7297,9 +7422,9 @@
   <mergeCells count="6">
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="A18:D18"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="E25:F25"/>
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <hyperlinks>
@@ -7331,24 +7456,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>341</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7440,11 +7565,11 @@
       <c r="A16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="49" t="s">
         <v>342</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
+      <c r="C16" s="50"/>
+      <c r="D16" s="51"/>
       <c r="E16" s="2" t="s">
         <v>17</v>
       </c>
@@ -7552,14 +7677,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>184</v>
@@ -7569,11 +7694,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7767,14 +7892,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14"/>
       <c r="F1" s="6" t="s">
         <v>184</v>
@@ -7784,11 +7909,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>441</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -7932,18 +8057,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>185</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8128,11 +8253,11 @@
       <c r="A24" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="49" t="s">
         <v>186</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="44"/>
+      <c r="C24" s="50"/>
+      <c r="D24" s="51"/>
       <c r="E24" s="2" t="s">
         <v>17</v>
       </c>
@@ -8226,18 +8351,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41"/>
-      <c r="B1" s="41"/>
+      <c r="A1" s="48"/>
+      <c r="B1" s="48"/>
     </row>
     <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>187</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8334,11 +8459,11 @@
       <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="42" t="s">
+      <c r="B15" s="49" t="s">
         <v>188</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="51"/>
       <c r="E15" s="2" t="s">
         <v>17</v>
       </c>
@@ -8427,14 +8552,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -8443,11 +8568,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>189</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8591,11 +8716,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>190</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -8693,14 +8818,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -8709,11 +8834,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>192</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -8832,11 +8957,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>191</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>
@@ -8952,14 +9077,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="48" t="s">
         <v>112</v>
       </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41" t="s">
+      <c r="B1" s="48"/>
+      <c r="C1" s="48" t="s">
         <v>113</v>
       </c>
-      <c r="D1" s="41"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="14">
         <v>41351</v>
       </c>
@@ -8968,11 +9093,11 @@
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="49" t="s">
         <v>193</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="44"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="51"/>
       <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
@@ -9080,11 +9205,11 @@
       <c r="A19" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="42" t="s">
+      <c r="B19" s="49" t="s">
         <v>194</v>
       </c>
-      <c r="C19" s="43"/>
-      <c r="D19" s="44"/>
+      <c r="C19" s="50"/>
+      <c r="D19" s="51"/>
       <c r="E19" s="2" t="s">
         <v>17</v>
       </c>

</xml_diff>

<commit_message>
complete #765: Error Parsing on Front End
</commit_message>
<xml_diff>
--- a/data_structure.xlsx
+++ b/data_structure.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670" firstSheet="16" activeTab="22"/>
+    <workbookView xWindow="120" yWindow="150" windowWidth="24915" windowHeight="12270" tabRatio="670"/>
   </bookViews>
   <sheets>
     <sheet name="Packages" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1517" uniqueCount="481">
   <si>
     <t>User Profile</t>
   </si>
@@ -1476,6 +1476,36 @@
   </si>
   <si>
     <t>image_height</t>
+  </si>
+  <si>
+    <t>find_my_club</t>
+  </si>
+  <si>
+    <t>registration/models/find_my_club</t>
+  </si>
+  <si>
+    <t>models/base</t>
+  </si>
+  <si>
+    <t>Get club information for the user</t>
+  </si>
+  <si>
+    <t>api/user/myclub</t>
+  </si>
+  <si>
+    <t>test/user/myclub</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>states</t>
+  </si>
+  <si>
+    <t>location/models/state</t>
+  </si>
+  <si>
+    <t>location/collections/states</t>
   </si>
 </sst>
 </file>
@@ -2066,13 +2096,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I32"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="C18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomRight" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2417,6 +2447,20 @@
       </c>
       <c r="C32" s="9" t="s">
         <v>141</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>477</v>
+      </c>
+      <c r="B34" s="9" t="s">
+        <v>478</v>
+      </c>
+      <c r="C34" s="9" t="s">
+        <v>479</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>480</v>
       </c>
     </row>
   </sheetData>
@@ -5247,13 +5291,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="F30" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="E41" sqref="E41"/>
+      <selection pane="bottomRight" activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6181,6 +6225,29 @@
       </c>
       <c r="K41" s="3" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
+        <v>471</v>
+      </c>
+      <c r="C42" s="9" t="s">
+        <v>472</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>473</v>
+      </c>
+      <c r="F42" s="9" t="s">
+        <v>474</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>475</v>
+      </c>
+      <c r="H42" s="9" t="s">
+        <v>476</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -7133,8 +7200,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>